<commit_message>
atualizando relação dos locais de de caixa fechada
</commit_message>
<xml_diff>
--- a/data/analise_curva_abc/local/datasets/local_apanha_cx.xlsx
+++ b/data/analise_curva_abc/local/datasets/local_apanha_cx.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\estoque\Documents\estoque.renan\projetos\projeto_curva_abc\analise_curva_abc\local\datasets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://maxifarmabr-my.sharepoint.com/personal/controle_estoque_grupomaxifarma_com_br/Documents/Documentos/estoque.renan/projetos/projeto_curva_abc/data/analise_curva_abc/local/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62563889-610E-48F9-917B-CDA4FE3D6C5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="13_ncr:1_{62563889-610E-48F9-917B-CDA4FE3D6C5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C1CEEF7D-F98E-424A-A29F-9429C7F5B664}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{18EFAD8D-C71D-455A-9E0F-2475F39BFCF9}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="964" uniqueCount="495">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="964" uniqueCount="492">
   <si>
     <t>local</t>
   </si>
@@ -1371,9 +1371,6 @@
     <t>018-038-00-02</t>
   </si>
   <si>
-    <t>fech_a</t>
-  </si>
-  <si>
     <t>014-006-02-01</t>
   </si>
   <si>
@@ -1485,21 +1482,9 @@
     <t>017-026-01-01</t>
   </si>
   <si>
-    <t>fech_bc</t>
-  </si>
-  <si>
-    <t>aberta_b</t>
-  </si>
-  <si>
-    <t>aberta_c</t>
-  </si>
-  <si>
     <t>ponta</t>
   </si>
   <si>
-    <t>flowrack</t>
-  </si>
-  <si>
     <t>antibiotico</t>
   </si>
   <si>
@@ -1513,6 +1498,12 @@
   </si>
   <si>
     <t>amostra</t>
+  </si>
+  <si>
+    <t>apanha_bc</t>
+  </si>
+  <si>
+    <t>apanha_a</t>
   </si>
 </sst>
 </file>
@@ -1597,9 +1588,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office 2013 - 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1637,7 +1628,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1743,7 +1734,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1885,7 +1876,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1896,7 +1887,7 @@
   <dimension ref="A1:B482"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B481" sqref="B481"/>
+      <selection activeCell="B111" sqref="B111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1927,7 +1918,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1935,7 +1926,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1943,7 +1934,7 @@
         <v>21</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1951,7 +1942,7 @@
         <v>28</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1959,7 +1950,7 @@
         <v>35</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1967,7 +1958,7 @@
         <v>42</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1975,7 +1966,7 @@
         <v>49</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1983,7 +1974,7 @@
         <v>56</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -1991,7 +1982,7 @@
         <v>63</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -1999,7 +1990,7 @@
         <v>70</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -2007,7 +1998,7 @@
         <v>77</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -2015,7 +2006,7 @@
         <v>84</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -2023,7 +2014,7 @@
         <v>92</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -2031,7 +2022,7 @@
         <v>100</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -2039,7 +2030,7 @@
         <v>106</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -2047,7 +2038,7 @@
         <v>113</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -2055,7 +2046,7 @@
         <v>120</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -2063,7 +2054,7 @@
         <v>127</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -2071,7 +2062,7 @@
         <v>134</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -2079,7 +2070,7 @@
         <v>141</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -2087,7 +2078,7 @@
         <v>148</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -2095,7 +2086,7 @@
         <v>155</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -2103,7 +2094,7 @@
         <v>162</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -2111,199 +2102,199 @@
         <v>169</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -2311,7 +2302,7 @@
         <v>234</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -2319,7 +2310,7 @@
         <v>239</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -2327,7 +2318,7 @@
         <v>244</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -2335,7 +2326,7 @@
         <v>249</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -2343,7 +2334,7 @@
         <v>253</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -2351,7 +2342,7 @@
         <v>257</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -2359,7 +2350,7 @@
         <v>261</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -2367,7 +2358,7 @@
         <v>265</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -2375,7 +2366,7 @@
         <v>269</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -2383,7 +2374,7 @@
         <v>273</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -2391,7 +2382,7 @@
         <v>277</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -2399,7 +2390,7 @@
         <v>281</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
@@ -2407,7 +2398,7 @@
         <v>284</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -2415,7 +2406,7 @@
         <v>287</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -2423,7 +2414,7 @@
         <v>290</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -2431,7 +2422,7 @@
         <v>293</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
@@ -2439,7 +2430,7 @@
         <v>296</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
@@ -2447,7 +2438,7 @@
         <v>299</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
@@ -2455,7 +2446,7 @@
         <v>302</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
@@ -2463,7 +2454,7 @@
         <v>305</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
@@ -2471,7 +2462,7 @@
         <v>308</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
@@ -2479,7 +2470,7 @@
         <v>311</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
@@ -2487,7 +2478,7 @@
         <v>313</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
@@ -2495,7 +2486,7 @@
         <v>315</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
@@ -2503,7 +2494,7 @@
         <v>317</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
@@ -2511,7 +2502,7 @@
         <v>319</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
@@ -2519,7 +2510,7 @@
         <v>321</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
@@ -2527,7 +2518,7 @@
         <v>323</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
@@ -2535,7 +2526,7 @@
         <v>325</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
@@ -2543,7 +2534,7 @@
         <v>327</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
@@ -2551,7 +2542,7 @@
         <v>329</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
@@ -2559,7 +2550,7 @@
         <v>331</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
@@ -2567,7 +2558,7 @@
         <v>333</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
@@ -2575,7 +2566,7 @@
         <v>335</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
@@ -2583,7 +2574,7 @@
         <v>337</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
@@ -2591,7 +2582,7 @@
         <v>339</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>447</v>
+        <v>491</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
@@ -2599,7 +2590,7 @@
         <v>341</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>447</v>
+        <v>485</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
@@ -2607,7 +2598,7 @@
         <v>343</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>447</v>
+        <v>485</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
@@ -2615,7 +2606,7 @@
         <v>345</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>447</v>
+        <v>485</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
@@ -2623,7 +2614,7 @@
         <v>347</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>447</v>
+        <v>485</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
@@ -2631,7 +2622,7 @@
         <v>349</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>447</v>
+        <v>485</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
@@ -2639,7 +2630,7 @@
         <v>351</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>447</v>
+        <v>485</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
@@ -2647,7 +2638,7 @@
         <v>353</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>447</v>
+        <v>485</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
@@ -2655,7 +2646,7 @@
         <v>355</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>447</v>
+        <v>485</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
@@ -2663,7 +2654,7 @@
         <v>357</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>447</v>
+        <v>485</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
@@ -2671,7 +2662,7 @@
         <v>359</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>447</v>
+        <v>485</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
@@ -2679,7 +2670,7 @@
         <v>361</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>447</v>
+        <v>485</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
@@ -2687,7 +2678,7 @@
         <v>363</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>447</v>
+        <v>485</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
@@ -2695,7 +2686,7 @@
         <v>365</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>447</v>
+        <v>485</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
@@ -2703,7 +2694,7 @@
         <v>367</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>447</v>
+        <v>485</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
@@ -2711,7 +2702,7 @@
         <v>369</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>447</v>
+        <v>485</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
@@ -2719,7 +2710,7 @@
         <v>371</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>447</v>
+        <v>485</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
@@ -2727,7 +2718,7 @@
         <v>373</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>447</v>
+        <v>485</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
@@ -2735,7 +2726,7 @@
         <v>375</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>447</v>
+        <v>485</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
@@ -2743,7 +2734,7 @@
         <v>376</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>447</v>
+        <v>485</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
@@ -2751,7 +2742,7 @@
         <v>377</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>447</v>
+        <v>485</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
@@ -2759,7 +2750,7 @@
         <v>378</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>447</v>
+        <v>485</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
@@ -2767,7 +2758,7 @@
         <v>379</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>447</v>
+        <v>485</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
@@ -2775,7 +2766,7 @@
         <v>380</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>447</v>
+        <v>485</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
@@ -2783,7 +2774,7 @@
         <v>381</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>447</v>
+        <v>485</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
@@ -2791,7 +2782,7 @@
         <v>382</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>447</v>
+        <v>485</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
@@ -2799,103 +2790,103 @@
         <v>383</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>447</v>
+        <v>485</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
@@ -2903,7 +2894,7 @@
         <v>85</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
@@ -2911,7 +2902,7 @@
         <v>93</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
@@ -2919,7 +2910,7 @@
         <v>101</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
@@ -2927,7 +2918,7 @@
         <v>107</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
@@ -2935,7 +2926,7 @@
         <v>114</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
@@ -2943,7 +2934,7 @@
         <v>121</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
@@ -2951,7 +2942,7 @@
         <v>128</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
@@ -2959,7 +2950,7 @@
         <v>135</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
@@ -2967,7 +2958,7 @@
         <v>142</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
@@ -2975,7 +2966,7 @@
         <v>149</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
@@ -2983,7 +2974,7 @@
         <v>156</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
@@ -2991,7 +2982,7 @@
         <v>163</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
@@ -2999,7 +2990,7 @@
         <v>170</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
@@ -3007,7 +2998,7 @@
         <v>175</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
@@ -3015,7 +3006,7 @@
         <v>180</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
@@ -3023,7 +3014,7 @@
         <v>185</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
@@ -3031,7 +3022,7 @@
         <v>190</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
@@ -3039,7 +3030,7 @@
         <v>195</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
@@ -3047,7 +3038,7 @@
         <v>200</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
@@ -3055,7 +3046,7 @@
         <v>205</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
@@ -3063,7 +3054,7 @@
         <v>210</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
@@ -3071,7 +3062,7 @@
         <v>215</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
@@ -3079,7 +3070,7 @@
         <v>220</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
@@ -3087,7 +3078,7 @@
         <v>225</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
@@ -3095,7 +3086,7 @@
         <v>230</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
@@ -3103,7 +3094,7 @@
         <v>235</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
@@ -3111,7 +3102,7 @@
         <v>240</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
@@ -3119,7 +3110,7 @@
         <v>245</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
@@ -3127,7 +3118,7 @@
         <v>250</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
@@ -3135,7 +3126,7 @@
         <v>254</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
@@ -3143,7 +3134,7 @@
         <v>258</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
@@ -3151,7 +3142,7 @@
         <v>262</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
@@ -3159,7 +3150,7 @@
         <v>266</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
@@ -3167,7 +3158,7 @@
         <v>270</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
@@ -3175,7 +3166,7 @@
         <v>274</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
@@ -3183,7 +3174,7 @@
         <v>278</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
@@ -3191,7 +3182,7 @@
         <v>282</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
@@ -3199,7 +3190,7 @@
         <v>285</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
@@ -3207,7 +3198,7 @@
         <v>288</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
@@ -3215,7 +3206,7 @@
         <v>291</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
@@ -3223,7 +3214,7 @@
         <v>294</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
@@ -3231,7 +3222,7 @@
         <v>297</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
@@ -3239,7 +3230,7 @@
         <v>300</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
@@ -3247,7 +3238,7 @@
         <v>303</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
@@ -3255,7 +3246,7 @@
         <v>306</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
@@ -3263,7 +3254,7 @@
         <v>309</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
@@ -3271,7 +3262,7 @@
         <v>312</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
@@ -3279,7 +3270,7 @@
         <v>314</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
@@ -3287,7 +3278,7 @@
         <v>316</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
@@ -3295,7 +3286,7 @@
         <v>318</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
@@ -3303,7 +3294,7 @@
         <v>320</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
@@ -3311,7 +3302,7 @@
         <v>322</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
@@ -3319,7 +3310,7 @@
         <v>324</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
@@ -3327,7 +3318,7 @@
         <v>326</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
@@ -3335,7 +3326,7 @@
         <v>328</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
@@ -3343,7 +3334,7 @@
         <v>330</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
@@ -3351,7 +3342,7 @@
         <v>332</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
@@ -3359,7 +3350,7 @@
         <v>334</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
@@ -3367,7 +3358,7 @@
         <v>336</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
@@ -3375,7 +3366,7 @@
         <v>338</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
@@ -3383,7 +3374,7 @@
         <v>340</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
@@ -3391,7 +3382,7 @@
         <v>342</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
@@ -3399,7 +3390,7 @@
         <v>344</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
@@ -3407,7 +3398,7 @@
         <v>346</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
@@ -3415,7 +3406,7 @@
         <v>348</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
@@ -3423,7 +3414,7 @@
         <v>350</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
@@ -3431,7 +3422,7 @@
         <v>352</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
@@ -3439,7 +3430,7 @@
         <v>354</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
@@ -3447,7 +3438,7 @@
         <v>356</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
@@ -3455,7 +3446,7 @@
         <v>358</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
@@ -3463,7 +3454,7 @@
         <v>360</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
@@ -3471,7 +3462,7 @@
         <v>362</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
@@ -3479,7 +3470,7 @@
         <v>364</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
@@ -3487,7 +3478,7 @@
         <v>366</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
@@ -3495,7 +3486,7 @@
         <v>368</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
@@ -3503,7 +3494,7 @@
         <v>370</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
@@ -3511,7 +3502,7 @@
         <v>372</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
@@ -3519,7 +3510,7 @@
         <v>374</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
@@ -3527,7 +3518,7 @@
         <v>1</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>485</v>
+        <v>490</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
@@ -3535,7 +3526,7 @@
         <v>8</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>485</v>
+        <v>490</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
@@ -3543,7 +3534,7 @@
         <v>15</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>485</v>
+        <v>490</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
@@ -3551,7 +3542,7 @@
         <v>22</v>
       </c>
       <c r="B205" s="1" t="s">
-        <v>485</v>
+        <v>490</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
@@ -3559,7 +3550,7 @@
         <v>29</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>485</v>
+        <v>490</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
@@ -3567,7 +3558,7 @@
         <v>36</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>485</v>
+        <v>490</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
@@ -3575,7 +3566,7 @@
         <v>43</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>485</v>
+        <v>490</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.25">
@@ -3583,7 +3574,7 @@
         <v>50</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>485</v>
+        <v>490</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.25">
@@ -3591,7 +3582,7 @@
         <v>57</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>485</v>
+        <v>490</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
@@ -3599,7 +3590,7 @@
         <v>64</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>485</v>
+        <v>490</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.25">
@@ -3607,7 +3598,7 @@
         <v>71</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>485</v>
+        <v>490</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.25">
@@ -3615,7 +3606,7 @@
         <v>78</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>485</v>
+        <v>490</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.25">
@@ -3623,7 +3614,7 @@
         <v>157</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>485</v>
+        <v>490</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.25">
@@ -3631,7 +3622,7 @@
         <v>164</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>485</v>
+        <v>490</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.25">
@@ -3639,7 +3630,7 @@
         <v>171</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>485</v>
+        <v>490</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.25">
@@ -3647,7 +3638,7 @@
         <v>176</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>485</v>
+        <v>490</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.25">
@@ -3655,7 +3646,7 @@
         <v>181</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>485</v>
+        <v>490</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.25">
@@ -3663,7 +3654,7 @@
         <v>186</v>
       </c>
       <c r="B219" s="1" t="s">
-        <v>485</v>
+        <v>490</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
@@ -3671,7 +3662,7 @@
         <v>191</v>
       </c>
       <c r="B220" s="1" t="s">
-        <v>485</v>
+        <v>490</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.25">
@@ -3679,7 +3670,7 @@
         <v>196</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>485</v>
+        <v>490</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.25">
@@ -3687,7 +3678,7 @@
         <v>201</v>
       </c>
       <c r="B222" s="1" t="s">
-        <v>485</v>
+        <v>490</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.25">
@@ -3695,7 +3686,7 @@
         <v>206</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>485</v>
+        <v>490</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.25">
@@ -3703,7 +3694,7 @@
         <v>211</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>485</v>
+        <v>490</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.25">
@@ -3711,7 +3702,7 @@
         <v>216</v>
       </c>
       <c r="B225" s="1" t="s">
-        <v>485</v>
+        <v>490</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.25">
@@ -3719,7 +3710,7 @@
         <v>221</v>
       </c>
       <c r="B226" s="1" t="s">
-        <v>485</v>
+        <v>490</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.25">
@@ -3727,7 +3718,7 @@
         <v>226</v>
       </c>
       <c r="B227" s="1" t="s">
-        <v>485</v>
+        <v>490</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.25">
@@ -3735,7 +3726,7 @@
         <v>231</v>
       </c>
       <c r="B228" s="1" t="s">
-        <v>485</v>
+        <v>490</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.25">
@@ -3743,7 +3734,7 @@
         <v>236</v>
       </c>
       <c r="B229" s="1" t="s">
-        <v>485</v>
+        <v>490</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.25">
@@ -3751,7 +3742,7 @@
         <v>241</v>
       </c>
       <c r="B230" s="1" t="s">
-        <v>485</v>
+        <v>490</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.25">
@@ -3759,7 +3750,7 @@
         <v>246</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>485</v>
+        <v>490</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.25">
@@ -3767,7 +3758,7 @@
         <v>251</v>
       </c>
       <c r="B232" s="1" t="s">
-        <v>485</v>
+        <v>490</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.25">
@@ -3775,7 +3766,7 @@
         <v>255</v>
       </c>
       <c r="B233" s="1" t="s">
-        <v>485</v>
+        <v>490</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.25">
@@ -3783,7 +3774,7 @@
         <v>259</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>485</v>
+        <v>490</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.25">
@@ -3791,7 +3782,7 @@
         <v>263</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>485</v>
+        <v>490</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.25">
@@ -3799,7 +3790,7 @@
         <v>267</v>
       </c>
       <c r="B236" s="1" t="s">
-        <v>485</v>
+        <v>490</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.25">
@@ -3807,7 +3798,7 @@
         <v>271</v>
       </c>
       <c r="B237" s="1" t="s">
-        <v>485</v>
+        <v>490</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.25">
@@ -3815,7 +3806,7 @@
         <v>275</v>
       </c>
       <c r="B238" s="1" t="s">
-        <v>485</v>
+        <v>490</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.25">
@@ -3823,7 +3814,7 @@
         <v>279</v>
       </c>
       <c r="B239" s="1" t="s">
-        <v>485</v>
+        <v>490</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.25">
@@ -3831,7 +3822,7 @@
         <v>283</v>
       </c>
       <c r="B240" s="1" t="s">
-        <v>485</v>
+        <v>490</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.25">
@@ -3839,7 +3830,7 @@
         <v>286</v>
       </c>
       <c r="B241" s="1" t="s">
-        <v>485</v>
+        <v>490</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.25">
@@ -3847,7 +3838,7 @@
         <v>289</v>
       </c>
       <c r="B242" s="1" t="s">
-        <v>485</v>
+        <v>490</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.25">
@@ -3855,7 +3846,7 @@
         <v>292</v>
       </c>
       <c r="B243" s="1" t="s">
-        <v>485</v>
+        <v>490</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.25">
@@ -3863,7 +3854,7 @@
         <v>295</v>
       </c>
       <c r="B244" s="1" t="s">
-        <v>485</v>
+        <v>490</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.25">
@@ -3871,7 +3862,7 @@
         <v>298</v>
       </c>
       <c r="B245" s="1" t="s">
-        <v>485</v>
+        <v>490</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.25">
@@ -3879,7 +3870,7 @@
         <v>301</v>
       </c>
       <c r="B246" s="1" t="s">
-        <v>485</v>
+        <v>490</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.25">
@@ -3887,7 +3878,7 @@
         <v>304</v>
       </c>
       <c r="B247" s="1" t="s">
-        <v>485</v>
+        <v>490</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.25">
@@ -3895,7 +3886,7 @@
         <v>307</v>
       </c>
       <c r="B248" s="1" t="s">
-        <v>485</v>
+        <v>490</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.25">
@@ -3903,391 +3894,391 @@
         <v>310</v>
       </c>
       <c r="B249" s="1" t="s">
-        <v>485</v>
+        <v>490</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A250" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B250" s="2" t="s">
-        <v>486</v>
+      <c r="B250" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A251" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B251" s="2" t="s">
-        <v>486</v>
+      <c r="B251" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A252" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B252" s="2" t="s">
-        <v>486</v>
+      <c r="B252" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A253" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B253" s="2" t="s">
-        <v>486</v>
+      <c r="B253" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A254" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B254" s="2" t="s">
-        <v>486</v>
+      <c r="B254" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A255" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B255" s="2" t="s">
-        <v>486</v>
+      <c r="B255" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A256" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B256" s="2" t="s">
-        <v>486</v>
+      <c r="B256" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A257" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B257" s="2" t="s">
-        <v>486</v>
+      <c r="B257" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A258" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B258" s="2" t="s">
-        <v>486</v>
+      <c r="B258" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A259" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B259" s="2" t="s">
-        <v>486</v>
+      <c r="B259" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A260" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B260" s="2" t="s">
-        <v>486</v>
+      <c r="B260" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A261" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B261" s="2" t="s">
-        <v>486</v>
+      <c r="B261" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A262" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B262" s="2" t="s">
-        <v>486</v>
+      <c r="B262" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A263" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B263" s="2" t="s">
-        <v>486</v>
+      <c r="B263" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A264" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B264" s="2" t="s">
-        <v>486</v>
+      <c r="B264" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A265" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B265" s="2" t="s">
-        <v>486</v>
+      <c r="B265" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A266" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B266" s="2" t="s">
-        <v>486</v>
+      <c r="B266" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A267" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B267" s="2" t="s">
-        <v>486</v>
+      <c r="B267" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A268" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B268" s="2" t="s">
-        <v>486</v>
+      <c r="B268" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A269" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B269" s="2" t="s">
-        <v>486</v>
+      <c r="B269" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A270" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B270" s="2" t="s">
-        <v>486</v>
+      <c r="B270" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A271" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="B271" s="2" t="s">
-        <v>486</v>
+      <c r="B271" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A272" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="B272" s="2" t="s">
-        <v>486</v>
+      <c r="B272" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A273" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="B273" s="2" t="s">
-        <v>486</v>
+      <c r="B273" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A274" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="B274" s="2" t="s">
-        <v>486</v>
+      <c r="B274" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A275" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="B275" s="2" t="s">
-        <v>486</v>
+      <c r="B275" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A276" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="B276" s="2" t="s">
-        <v>486</v>
+      <c r="B276" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A277" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="B277" s="2" t="s">
-        <v>486</v>
+      <c r="B277" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A278" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="B278" s="2" t="s">
-        <v>486</v>
+      <c r="B278" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A279" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="B279" s="2" t="s">
-        <v>486</v>
+      <c r="B279" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A280" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="B280" s="2" t="s">
-        <v>486</v>
+      <c r="B280" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A281" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="B281" s="2" t="s">
-        <v>486</v>
+      <c r="B281" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A282" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="B282" s="2" t="s">
-        <v>486</v>
+      <c r="B282" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A283" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="B283" s="2" t="s">
-        <v>486</v>
+      <c r="B283" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A284" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="B284" s="2" t="s">
-        <v>486</v>
+      <c r="B284" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A285" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="B285" s="2" t="s">
-        <v>486</v>
+      <c r="B285" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A286" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="B286" s="2" t="s">
-        <v>486</v>
+      <c r="B286" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A287" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="B287" s="2" t="s">
-        <v>486</v>
+      <c r="B287" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A288" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="B288" s="2" t="s">
-        <v>486</v>
+      <c r="B288" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A289" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="B289" s="2" t="s">
-        <v>486</v>
+      <c r="B289" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A290" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="B290" s="2" t="s">
-        <v>486</v>
+      <c r="B290" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A291" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="B291" s="2" t="s">
-        <v>486</v>
+      <c r="B291" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A292" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="B292" s="2" t="s">
-        <v>486</v>
+      <c r="B292" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A293" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="B293" s="2" t="s">
-        <v>486</v>
+      <c r="B293" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A294" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="B294" s="2" t="s">
-        <v>486</v>
+      <c r="B294" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A295" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="B295" s="2" t="s">
-        <v>486</v>
+      <c r="B295" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A296" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="B296" s="2" t="s">
-        <v>486</v>
+      <c r="B296" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="297" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A297" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="B297" s="2" t="s">
-        <v>486</v>
+      <c r="B297" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.25">
@@ -4295,7 +4286,7 @@
         <v>4</v>
       </c>
       <c r="B298" s="2" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.25">
@@ -4303,7 +4294,7 @@
         <v>11</v>
       </c>
       <c r="B299" s="2" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.25">
@@ -4311,7 +4302,7 @@
         <v>18</v>
       </c>
       <c r="B300" s="2" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.25">
@@ -4319,7 +4310,7 @@
         <v>25</v>
       </c>
       <c r="B301" s="2" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.25">
@@ -4327,7 +4318,7 @@
         <v>32</v>
       </c>
       <c r="B302" s="2" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.25">
@@ -4335,7 +4326,7 @@
         <v>39</v>
       </c>
       <c r="B303" s="2" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
     </row>
     <row r="304" spans="1:2" x14ac:dyDescent="0.25">
@@ -4343,7 +4334,7 @@
         <v>46</v>
       </c>
       <c r="B304" s="2" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.25">
@@ -4351,7 +4342,7 @@
         <v>53</v>
       </c>
       <c r="B305" s="2" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
     </row>
     <row r="306" spans="1:2" x14ac:dyDescent="0.25">
@@ -4359,7 +4350,7 @@
         <v>60</v>
       </c>
       <c r="B306" s="2" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
     </row>
     <row r="307" spans="1:2" x14ac:dyDescent="0.25">
@@ -4367,7 +4358,7 @@
         <v>67</v>
       </c>
       <c r="B307" s="2" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
     </row>
     <row r="308" spans="1:2" x14ac:dyDescent="0.25">
@@ -4375,7 +4366,7 @@
         <v>74</v>
       </c>
       <c r="B308" s="2" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
     </row>
     <row r="309" spans="1:2" x14ac:dyDescent="0.25">
@@ -4383,7 +4374,7 @@
         <v>81</v>
       </c>
       <c r="B309" s="2" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
     </row>
     <row r="310" spans="1:2" x14ac:dyDescent="0.25">
@@ -4391,7 +4382,7 @@
         <v>89</v>
       </c>
       <c r="B310" s="2" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
     </row>
     <row r="311" spans="1:2" x14ac:dyDescent="0.25">
@@ -4399,7 +4390,7 @@
         <v>97</v>
       </c>
       <c r="B311" s="2" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.25">
@@ -4407,7 +4398,7 @@
         <v>97</v>
       </c>
       <c r="B312" s="2" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
     </row>
     <row r="313" spans="1:2" x14ac:dyDescent="0.25">
@@ -4415,7 +4406,7 @@
         <v>111</v>
       </c>
       <c r="B313" s="2" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
     </row>
     <row r="314" spans="1:2" x14ac:dyDescent="0.25">
@@ -4423,7 +4414,7 @@
         <v>118</v>
       </c>
       <c r="B314" s="2" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
     </row>
     <row r="315" spans="1:2" x14ac:dyDescent="0.25">
@@ -4431,7 +4422,7 @@
         <v>125</v>
       </c>
       <c r="B315" s="2" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
     </row>
     <row r="316" spans="1:2" x14ac:dyDescent="0.25">
@@ -4439,7 +4430,7 @@
         <v>132</v>
       </c>
       <c r="B316" s="2" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
     </row>
     <row r="317" spans="1:2" x14ac:dyDescent="0.25">
@@ -4447,7 +4438,7 @@
         <v>139</v>
       </c>
       <c r="B317" s="2" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
     </row>
     <row r="318" spans="1:2" x14ac:dyDescent="0.25">
@@ -4455,7 +4446,7 @@
         <v>146</v>
       </c>
       <c r="B318" s="2" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
     </row>
     <row r="319" spans="1:2" x14ac:dyDescent="0.25">
@@ -4463,7 +4454,7 @@
         <v>153</v>
       </c>
       <c r="B319" s="2" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
     </row>
     <row r="320" spans="1:2" x14ac:dyDescent="0.25">
@@ -4471,7 +4462,7 @@
         <v>160</v>
       </c>
       <c r="B320" s="2" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
     </row>
     <row r="321" spans="1:2" x14ac:dyDescent="0.25">
@@ -4479,7 +4470,7 @@
         <v>167</v>
       </c>
       <c r="B321" s="2" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.25">
@@ -4487,7 +4478,7 @@
         <v>174</v>
       </c>
       <c r="B322" s="2" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
     </row>
     <row r="323" spans="1:2" x14ac:dyDescent="0.25">
@@ -4495,7 +4486,7 @@
         <v>179</v>
       </c>
       <c r="B323" s="2" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
     </row>
     <row r="324" spans="1:2" x14ac:dyDescent="0.25">
@@ -4503,7 +4494,7 @@
         <v>184</v>
       </c>
       <c r="B324" s="2" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
     </row>
     <row r="325" spans="1:2" x14ac:dyDescent="0.25">
@@ -4511,7 +4502,7 @@
         <v>189</v>
       </c>
       <c r="B325" s="2" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
     </row>
     <row r="326" spans="1:2" x14ac:dyDescent="0.25">
@@ -4519,7 +4510,7 @@
         <v>194</v>
       </c>
       <c r="B326" s="2" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
     </row>
     <row r="327" spans="1:2" x14ac:dyDescent="0.25">
@@ -4527,7 +4518,7 @@
         <v>199</v>
       </c>
       <c r="B327" s="2" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
     </row>
     <row r="328" spans="1:2" x14ac:dyDescent="0.25">
@@ -4535,7 +4526,7 @@
         <v>204</v>
       </c>
       <c r="B328" s="2" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
     </row>
     <row r="329" spans="1:2" x14ac:dyDescent="0.25">
@@ -4543,7 +4534,7 @@
         <v>209</v>
       </c>
       <c r="B329" s="2" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
     </row>
     <row r="330" spans="1:2" x14ac:dyDescent="0.25">
@@ -4551,7 +4542,7 @@
         <v>214</v>
       </c>
       <c r="B330" s="2" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
     </row>
     <row r="331" spans="1:2" x14ac:dyDescent="0.25">
@@ -4559,7 +4550,7 @@
         <v>219</v>
       </c>
       <c r="B331" s="2" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
     </row>
     <row r="332" spans="1:2" x14ac:dyDescent="0.25">
@@ -4567,7 +4558,7 @@
         <v>224</v>
       </c>
       <c r="B332" s="2" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
     </row>
     <row r="333" spans="1:2" x14ac:dyDescent="0.25">
@@ -4575,407 +4566,407 @@
         <v>229</v>
       </c>
       <c r="B333" s="2" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
     </row>
     <row r="334" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A334" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B334" s="2" t="s">
-        <v>487</v>
+      <c r="B334" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="335" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A335" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B335" s="2" t="s">
-        <v>487</v>
+      <c r="B335" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="336" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A336" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B336" s="2" t="s">
-        <v>487</v>
+      <c r="B336" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="337" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A337" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B337" s="2" t="s">
-        <v>487</v>
+      <c r="B337" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="338" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A338" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B338" s="2" t="s">
-        <v>487</v>
+      <c r="B338" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="339" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A339" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B339" s="2" t="s">
-        <v>487</v>
+      <c r="B339" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="340" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A340" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B340" s="2" t="s">
-        <v>487</v>
+      <c r="B340" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="341" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A341" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B341" s="2" t="s">
-        <v>487</v>
+      <c r="B341" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="342" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A342" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B342" s="2" t="s">
-        <v>487</v>
+      <c r="B342" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="343" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A343" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B343" s="2" t="s">
-        <v>487</v>
+      <c r="B343" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="344" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A344" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B344" s="2" t="s">
-        <v>487</v>
+      <c r="B344" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="345" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A345" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B345" s="2" t="s">
-        <v>487</v>
+      <c r="B345" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="346" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A346" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B346" s="2" t="s">
-        <v>487</v>
+      <c r="B346" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="347" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A347" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B347" s="2" t="s">
-        <v>487</v>
+      <c r="B347" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="348" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A348" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B348" s="2" t="s">
-        <v>487</v>
+      <c r="B348" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="349" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A349" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B349" s="2" t="s">
-        <v>487</v>
+      <c r="B349" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="350" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A350" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B350" s="2" t="s">
-        <v>487</v>
+      <c r="B350" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A351" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B351" s="2" t="s">
-        <v>487</v>
+      <c r="B351" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="352" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A352" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B352" s="2" t="s">
-        <v>487</v>
+      <c r="B352" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="353" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A353" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B353" s="2" t="s">
-        <v>487</v>
+      <c r="B353" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="354" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A354" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B354" s="2" t="s">
-        <v>487</v>
+      <c r="B354" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="355" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A355" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="B355" s="2" t="s">
-        <v>487</v>
+      <c r="B355" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="356" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A356" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="B356" s="2" t="s">
-        <v>487</v>
+      <c r="B356" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="357" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A357" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B357" s="2" t="s">
-        <v>487</v>
+      <c r="B357" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="358" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A358" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="B358" s="2" t="s">
-        <v>487</v>
+      <c r="B358" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="359" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A359" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="B359" s="2" t="s">
-        <v>487</v>
+      <c r="B359" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="360" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A360" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="B360" s="2" t="s">
-        <v>487</v>
+      <c r="B360" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="361" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A361" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="B361" s="2" t="s">
-        <v>487</v>
+      <c r="B361" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="362" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A362" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B362" s="2" t="s">
-        <v>487</v>
+      <c r="B362" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="363" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A363" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="B363" s="2" t="s">
-        <v>487</v>
+      <c r="B363" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="364" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A364" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="B364" s="2" t="s">
-        <v>487</v>
+      <c r="B364" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="365" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A365" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="B365" s="2" t="s">
-        <v>487</v>
+      <c r="B365" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="366" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A366" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="B366" s="2" t="s">
-        <v>487</v>
+      <c r="B366" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="367" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A367" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="B367" s="2" t="s">
-        <v>487</v>
+      <c r="B367" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A368" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="B368" s="2" t="s">
-        <v>487</v>
+      <c r="B368" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="369" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A369" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="B369" s="2" t="s">
-        <v>487</v>
+      <c r="B369" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="370" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A370" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="B370" s="2" t="s">
-        <v>487</v>
+      <c r="B370" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="371" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A371" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="B371" s="2" t="s">
-        <v>487</v>
+      <c r="B371" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A372" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="B372" s="2" t="s">
-        <v>487</v>
+      <c r="B372" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="373" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A373" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="B373" s="2" t="s">
-        <v>487</v>
+      <c r="B373" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A374" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B374" s="2" t="s">
-        <v>485</v>
+      <c r="B374" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="375" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A375" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B375" s="2" t="s">
-        <v>485</v>
+      <c r="B375" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A376" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B376" s="2" t="s">
-        <v>485</v>
+      <c r="B376" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="377" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A377" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B377" s="2" t="s">
-        <v>485</v>
+      <c r="B377" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="378" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A378" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B378" s="2" t="s">
-        <v>485</v>
+      <c r="B378" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A379" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B379" s="2" t="s">
-        <v>485</v>
+      <c r="B379" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="380" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A380" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B380" s="2" t="s">
-        <v>485</v>
+      <c r="B380" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="381" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A381" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B381" s="2" t="s">
-        <v>485</v>
+      <c r="B381" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A382" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B382" s="2" t="s">
-        <v>485</v>
+      <c r="B382" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="383" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A383" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B383" s="2" t="s">
-        <v>485</v>
+      <c r="B383" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="384" spans="1:2" x14ac:dyDescent="0.25">
@@ -4983,7 +4974,7 @@
         <v>384</v>
       </c>
       <c r="B384" s="2" t="s">
-        <v>491</v>
+        <v>486</v>
       </c>
     </row>
     <row r="385" spans="1:2" x14ac:dyDescent="0.25">
@@ -4991,7 +4982,7 @@
         <v>385</v>
       </c>
       <c r="B385" s="2" t="s">
-        <v>491</v>
+        <v>486</v>
       </c>
     </row>
     <row r="386" spans="1:2" x14ac:dyDescent="0.25">
@@ -4999,7 +4990,7 @@
         <v>386</v>
       </c>
       <c r="B386" s="2" t="s">
-        <v>491</v>
+        <v>486</v>
       </c>
     </row>
     <row r="387" spans="1:2" x14ac:dyDescent="0.25">
@@ -5007,7 +4998,7 @@
         <v>387</v>
       </c>
       <c r="B387" s="2" t="s">
-        <v>491</v>
+        <v>486</v>
       </c>
     </row>
     <row r="388" spans="1:2" x14ac:dyDescent="0.25">
@@ -5015,7 +5006,7 @@
         <v>388</v>
       </c>
       <c r="B388" s="2" t="s">
-        <v>491</v>
+        <v>486</v>
       </c>
     </row>
     <row r="389" spans="1:2" x14ac:dyDescent="0.25">
@@ -5023,7 +5014,7 @@
         <v>389</v>
       </c>
       <c r="B389" s="2" t="s">
-        <v>491</v>
+        <v>486</v>
       </c>
     </row>
     <row r="390" spans="1:2" x14ac:dyDescent="0.25">
@@ -5031,7 +5022,7 @@
         <v>390</v>
       </c>
       <c r="B390" s="2" t="s">
-        <v>491</v>
+        <v>486</v>
       </c>
     </row>
     <row r="391" spans="1:2" x14ac:dyDescent="0.25">
@@ -5039,7 +5030,7 @@
         <v>391</v>
       </c>
       <c r="B391" s="2" t="s">
-        <v>491</v>
+        <v>486</v>
       </c>
     </row>
     <row r="392" spans="1:2" x14ac:dyDescent="0.25">
@@ -5047,7 +5038,7 @@
         <v>392</v>
       </c>
       <c r="B392" s="2" t="s">
-        <v>491</v>
+        <v>486</v>
       </c>
     </row>
     <row r="393" spans="1:2" x14ac:dyDescent="0.25">
@@ -5055,7 +5046,7 @@
         <v>393</v>
       </c>
       <c r="B393" s="2" t="s">
-        <v>491</v>
+        <v>486</v>
       </c>
     </row>
     <row r="394" spans="1:2" x14ac:dyDescent="0.25">
@@ -5063,7 +5054,7 @@
         <v>394</v>
       </c>
       <c r="B394" s="2" t="s">
-        <v>491</v>
+        <v>486</v>
       </c>
     </row>
     <row r="395" spans="1:2" x14ac:dyDescent="0.25">
@@ -5071,199 +5062,199 @@
         <v>395</v>
       </c>
       <c r="B395" s="2" t="s">
-        <v>491</v>
+        <v>486</v>
       </c>
     </row>
     <row r="396" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A396" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B396" s="2" t="s">
-        <v>489</v>
+      <c r="B396" s="1" t="s">
+        <v>491</v>
       </c>
     </row>
     <row r="397" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A397" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B397" s="2" t="s">
-        <v>489</v>
+      <c r="B397" s="1" t="s">
+        <v>491</v>
       </c>
     </row>
     <row r="398" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A398" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B398" s="2" t="s">
-        <v>489</v>
+      <c r="B398" s="1" t="s">
+        <v>491</v>
       </c>
     </row>
     <row r="399" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A399" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B399" s="2" t="s">
-        <v>489</v>
+      <c r="B399" s="1" t="s">
+        <v>491</v>
       </c>
     </row>
     <row r="400" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A400" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B400" s="2" t="s">
-        <v>489</v>
+      <c r="B400" s="1" t="s">
+        <v>491</v>
       </c>
     </row>
     <row r="401" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A401" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B401" s="2" t="s">
-        <v>489</v>
+      <c r="B401" s="1" t="s">
+        <v>491</v>
       </c>
     </row>
     <row r="402" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A402" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B402" s="2" t="s">
-        <v>489</v>
+      <c r="B402" s="1" t="s">
+        <v>491</v>
       </c>
     </row>
     <row r="403" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A403" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B403" s="2" t="s">
-        <v>489</v>
+      <c r="B403" s="1" t="s">
+        <v>491</v>
       </c>
     </row>
     <row r="404" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A404" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B404" s="2" t="s">
-        <v>489</v>
+      <c r="B404" s="1" t="s">
+        <v>491</v>
       </c>
     </row>
     <row r="405" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A405" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B405" s="2" t="s">
-        <v>489</v>
+      <c r="B405" s="1" t="s">
+        <v>491</v>
       </c>
     </row>
     <row r="406" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A406" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B406" s="2" t="s">
-        <v>489</v>
+      <c r="B406" s="1" t="s">
+        <v>491</v>
       </c>
     </row>
     <row r="407" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A407" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B407" s="2" t="s">
-        <v>489</v>
+      <c r="B407" s="1" t="s">
+        <v>491</v>
       </c>
     </row>
     <row r="408" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A408" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B408" s="2" t="s">
-        <v>489</v>
+      <c r="B408" s="1" t="s">
+        <v>491</v>
       </c>
     </row>
     <row r="409" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A409" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B409" s="2" t="s">
-        <v>489</v>
+      <c r="B409" s="1" t="s">
+        <v>491</v>
       </c>
     </row>
     <row r="410" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A410" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B410" s="2" t="s">
-        <v>489</v>
+      <c r="B410" s="1" t="s">
+        <v>491</v>
       </c>
     </row>
     <row r="411" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A411" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B411" s="2" t="s">
-        <v>489</v>
+      <c r="B411" s="1" t="s">
+        <v>491</v>
       </c>
     </row>
     <row r="412" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A412" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B412" s="2" t="s">
-        <v>489</v>
+      <c r="B412" s="1" t="s">
+        <v>491</v>
       </c>
     </row>
     <row r="413" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A413" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B413" s="2" t="s">
-        <v>489</v>
+      <c r="B413" s="1" t="s">
+        <v>491</v>
       </c>
     </row>
     <row r="414" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A414" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B414" s="2" t="s">
-        <v>489</v>
+      <c r="B414" s="1" t="s">
+        <v>491</v>
       </c>
     </row>
     <row r="415" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A415" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B415" s="2" t="s">
-        <v>489</v>
+      <c r="B415" s="1" t="s">
+        <v>491</v>
       </c>
     </row>
     <row r="416" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A416" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="B416" s="2" t="s">
-        <v>489</v>
+      <c r="B416" s="1" t="s">
+        <v>491</v>
       </c>
     </row>
     <row r="417" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A417" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="B417" s="2" t="s">
-        <v>489</v>
+      <c r="B417" s="1" t="s">
+        <v>491</v>
       </c>
     </row>
     <row r="418" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A418" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="B418" s="2" t="s">
-        <v>489</v>
+      <c r="B418" s="1" t="s">
+        <v>491</v>
       </c>
     </row>
     <row r="419" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A419" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="B419" s="2" t="s">
-        <v>489</v>
+      <c r="B419" s="1" t="s">
+        <v>491</v>
       </c>
     </row>
     <row r="420" spans="1:2" x14ac:dyDescent="0.25">
@@ -5383,7 +5374,7 @@
         <v>414</v>
       </c>
       <c r="B434" s="1" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
     </row>
     <row r="435" spans="1:2" x14ac:dyDescent="0.25">
@@ -5391,7 +5382,7 @@
         <v>415</v>
       </c>
       <c r="B435" s="1" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
     </row>
     <row r="436" spans="1:2" x14ac:dyDescent="0.25">
@@ -5399,7 +5390,7 @@
         <v>416</v>
       </c>
       <c r="B436" s="1" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
     </row>
     <row r="437" spans="1:2" x14ac:dyDescent="0.25">
@@ -5407,7 +5398,7 @@
         <v>417</v>
       </c>
       <c r="B437" s="1" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
     </row>
     <row r="438" spans="1:2" x14ac:dyDescent="0.25">
@@ -5415,7 +5406,7 @@
         <v>418</v>
       </c>
       <c r="B438" s="1" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
     </row>
     <row r="439" spans="1:2" x14ac:dyDescent="0.25">
@@ -5423,7 +5414,7 @@
         <v>419</v>
       </c>
       <c r="B439" s="1" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
     </row>
     <row r="440" spans="1:2" x14ac:dyDescent="0.25">
@@ -5431,7 +5422,7 @@
         <v>420</v>
       </c>
       <c r="B440" s="1" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
     </row>
     <row r="441" spans="1:2" x14ac:dyDescent="0.25">
@@ -5439,7 +5430,7 @@
         <v>421</v>
       </c>
       <c r="B441" s="1" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
     </row>
     <row r="442" spans="1:2" x14ac:dyDescent="0.25">
@@ -5447,7 +5438,7 @@
         <v>422</v>
       </c>
       <c r="B442" s="1" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
     </row>
     <row r="443" spans="1:2" x14ac:dyDescent="0.25">
@@ -5455,7 +5446,7 @@
         <v>423</v>
       </c>
       <c r="B443" s="1" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
     </row>
     <row r="444" spans="1:2" x14ac:dyDescent="0.25">
@@ -5463,7 +5454,7 @@
         <v>424</v>
       </c>
       <c r="B444" s="1" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
     </row>
     <row r="445" spans="1:2" x14ac:dyDescent="0.25">
@@ -5471,7 +5462,7 @@
         <v>425</v>
       </c>
       <c r="B445" s="1" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
     </row>
     <row r="446" spans="1:2" x14ac:dyDescent="0.25">
@@ -5479,7 +5470,7 @@
         <v>426</v>
       </c>
       <c r="B446" s="1" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
     </row>
     <row r="447" spans="1:2" x14ac:dyDescent="0.25">
@@ -5487,7 +5478,7 @@
         <v>427</v>
       </c>
       <c r="B447" s="1" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
     </row>
     <row r="448" spans="1:2" x14ac:dyDescent="0.25">
@@ -5495,7 +5486,7 @@
         <v>428</v>
       </c>
       <c r="B448" s="1" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
     </row>
     <row r="449" spans="1:2" x14ac:dyDescent="0.25">
@@ -5503,7 +5494,7 @@
         <v>429</v>
       </c>
       <c r="B449" s="1" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
     </row>
     <row r="450" spans="1:2" x14ac:dyDescent="0.25">
@@ -5511,7 +5502,7 @@
         <v>430</v>
       </c>
       <c r="B450" s="1" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
     </row>
     <row r="451" spans="1:2" x14ac:dyDescent="0.25">
@@ -5519,7 +5510,7 @@
         <v>431</v>
       </c>
       <c r="B451" s="1" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
     </row>
     <row r="452" spans="1:2" x14ac:dyDescent="0.25">
@@ -5527,7 +5518,7 @@
         <v>432</v>
       </c>
       <c r="B452" s="1" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
     </row>
     <row r="453" spans="1:2" x14ac:dyDescent="0.25">
@@ -5535,7 +5526,7 @@
         <v>433</v>
       </c>
       <c r="B453" s="1" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
     </row>
     <row r="454" spans="1:2" x14ac:dyDescent="0.25">
@@ -5543,7 +5534,7 @@
         <v>434</v>
       </c>
       <c r="B454" s="1" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
     </row>
     <row r="455" spans="1:2" x14ac:dyDescent="0.25">
@@ -5551,7 +5542,7 @@
         <v>435</v>
       </c>
       <c r="B455" s="1" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
     </row>
     <row r="456" spans="1:2" x14ac:dyDescent="0.25">
@@ -5559,7 +5550,7 @@
         <v>436</v>
       </c>
       <c r="B456" s="1" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
     </row>
     <row r="457" spans="1:2" x14ac:dyDescent="0.25">
@@ -5567,7 +5558,7 @@
         <v>437</v>
       </c>
       <c r="B457" s="1" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
     </row>
     <row r="458" spans="1:2" x14ac:dyDescent="0.25">
@@ -5575,7 +5566,7 @@
         <v>438</v>
       </c>
       <c r="B458" s="1" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
     </row>
     <row r="459" spans="1:2" x14ac:dyDescent="0.25">
@@ -5583,7 +5574,7 @@
         <v>439</v>
       </c>
       <c r="B459" s="1" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
     </row>
     <row r="460" spans="1:2" x14ac:dyDescent="0.25">
@@ -5591,7 +5582,7 @@
         <v>440</v>
       </c>
       <c r="B460" s="1" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
     </row>
     <row r="461" spans="1:2" x14ac:dyDescent="0.25">
@@ -5599,7 +5590,7 @@
         <v>441</v>
       </c>
       <c r="B461" s="1" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
     </row>
     <row r="462" spans="1:2" x14ac:dyDescent="0.25">
@@ -5607,7 +5598,7 @@
         <v>442</v>
       </c>
       <c r="B462" s="1" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
     </row>
     <row r="463" spans="1:2" x14ac:dyDescent="0.25">
@@ -5615,7 +5606,7 @@
         <v>443</v>
       </c>
       <c r="B463" s="1" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
     </row>
     <row r="464" spans="1:2" x14ac:dyDescent="0.25">
@@ -5623,7 +5614,7 @@
         <v>444</v>
       </c>
       <c r="B464" s="1" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
     </row>
     <row r="465" spans="1:2" x14ac:dyDescent="0.25">
@@ -5631,7 +5622,7 @@
         <v>445</v>
       </c>
       <c r="B465" s="1" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
     </row>
     <row r="466" spans="1:2" x14ac:dyDescent="0.25">
@@ -5639,7 +5630,7 @@
         <v>446</v>
       </c>
       <c r="B466" s="1" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
     </row>
     <row r="467" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Adicionando endereço faltante na relação
</commit_message>
<xml_diff>
--- a/data/analise_curva_abc/local/datasets/local_apanha_cx.xlsx
+++ b/data/analise_curva_abc/local/datasets/local_apanha_cx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://maxifarmabr-my.sharepoint.com/personal/controle_estoque_grupomaxifarma_com_br/Documents/Documentos/estoque.renan/projetos/projeto_curva_abc/data/analise_curva_abc/local/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="46" documentId="13_ncr:1_{62563889-610E-48F9-917B-CDA4FE3D6C5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1A3CB8FB-B6CE-42D3-8DFD-ADA84DBF6FD3}"/>
+  <xr:revisionPtr revIDLastSave="55" documentId="13_ncr:1_{62563889-610E-48F9-917B-CDA4FE3D6C5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B1D9B4B8-C6BA-4293-9939-1EF7C6A4E335}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{18EFAD8D-C71D-455A-9E0F-2475F39BFCF9}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$1:$B$482</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$1:$B$483</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="964" uniqueCount="493">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="966" uniqueCount="494">
   <si>
     <t>local</t>
   </si>
@@ -1507,13 +1507,16 @@
   </si>
   <si>
     <t>apanha_c</t>
+  </si>
+  <si>
+    <t>010-042-01-01</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1524,6 +1527,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1564,7 +1575,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1573,6 +1584,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1891,29 +1903,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3722E28-546D-45F9-BF38-B4D5FA1D8738}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:B482"/>
+  <dimension ref="A1:D483"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B209" sqref="B209"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>396</v>
       </c>
@@ -1921,7 +1923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -1929,7 +1931,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="3" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -1937,7 +1939,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="4" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
@@ -1945,7 +1947,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="5" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>28</v>
       </c>
@@ -1953,7 +1955,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="6" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>35</v>
       </c>
@@ -1961,7 +1963,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="7" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>42</v>
       </c>
@@ -1969,7 +1971,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="8" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>49</v>
       </c>
@@ -1977,7 +1979,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="9" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>56</v>
       </c>
@@ -1985,15 +1987,16 @@
         <v>490</v>
       </c>
     </row>
-    <row r="10" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>63</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>490</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>70</v>
       </c>
@@ -2001,7 +2004,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="12" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>77</v>
       </c>
@@ -2009,7 +2012,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="13" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>84</v>
       </c>
@@ -2017,7 +2020,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="14" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>92</v>
       </c>
@@ -2025,7 +2028,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="15" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>100</v>
       </c>
@@ -2033,7 +2036,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="16" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>106</v>
       </c>
@@ -2041,7 +2044,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="17" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>113</v>
       </c>
@@ -2049,7 +2052,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="18" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>120</v>
       </c>
@@ -2057,7 +2060,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="19" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>127</v>
       </c>
@@ -2065,7 +2068,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="20" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>134</v>
       </c>
@@ -2073,7 +2076,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="21" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>141</v>
       </c>
@@ -2081,7 +2084,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="22" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>148</v>
       </c>
@@ -2089,7 +2092,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="23" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>155</v>
       </c>
@@ -2097,7 +2100,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="24" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>162</v>
       </c>
@@ -2105,7 +2108,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="25" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>169</v>
       </c>
@@ -2113,7 +2116,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="26" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>447</v>
       </c>
@@ -2121,7 +2124,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="27" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>448</v>
       </c>
@@ -2129,7 +2132,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="28" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>449</v>
       </c>
@@ -2137,7 +2140,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="29" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>450</v>
       </c>
@@ -2145,7 +2148,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="30" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>451</v>
       </c>
@@ -2153,7 +2156,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="31" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>452</v>
       </c>
@@ -2161,7 +2164,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="32" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>453</v>
       </c>
@@ -2169,7 +2172,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="33" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>454</v>
       </c>
@@ -2177,7 +2180,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="34" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>455</v>
       </c>
@@ -2185,7 +2188,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="35" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>456</v>
       </c>
@@ -2193,7 +2196,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="36" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>457</v>
       </c>
@@ -2201,7 +2204,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="37" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>458</v>
       </c>
@@ -2209,7 +2212,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="38" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>459</v>
       </c>
@@ -2217,7 +2220,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="39" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>460</v>
       </c>
@@ -2225,7 +2228,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="40" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>461</v>
       </c>
@@ -2233,7 +2236,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="41" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>462</v>
       </c>
@@ -2241,7 +2244,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="42" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>463</v>
       </c>
@@ -2249,7 +2252,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="43" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>464</v>
       </c>
@@ -2257,7 +2260,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="44" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>465</v>
       </c>
@@ -2265,7 +2268,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="45" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>466</v>
       </c>
@@ -2273,7 +2276,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="46" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>467</v>
       </c>
@@ -2281,7 +2284,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="47" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>468</v>
       </c>
@@ -2289,7 +2292,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="48" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>469</v>
       </c>
@@ -2297,7 +2300,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="49" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>470</v>
       </c>
@@ -2305,7 +2308,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="50" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>234</v>
       </c>
@@ -2313,7 +2316,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="51" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>239</v>
       </c>
@@ -2321,7 +2324,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="52" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>244</v>
       </c>
@@ -2329,7 +2332,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="53" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>249</v>
       </c>
@@ -2337,7 +2340,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="54" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>253</v>
       </c>
@@ -2345,7 +2348,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="55" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>257</v>
       </c>
@@ -2353,7 +2356,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="56" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>261</v>
       </c>
@@ -2361,7 +2364,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="57" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>265</v>
       </c>
@@ -2369,7 +2372,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="58" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>269</v>
       </c>
@@ -2377,7 +2380,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="59" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>273</v>
       </c>
@@ -2385,7 +2388,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="60" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>277</v>
       </c>
@@ -2393,7 +2396,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="61" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>281</v>
       </c>
@@ -2401,7 +2404,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="62" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>284</v>
       </c>
@@ -2409,7 +2412,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="63" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>287</v>
       </c>
@@ -2417,7 +2420,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="64" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>290</v>
       </c>
@@ -2425,7 +2428,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="65" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>293</v>
       </c>
@@ -2433,7 +2436,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="66" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>296</v>
       </c>
@@ -2441,7 +2444,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="67" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>299</v>
       </c>
@@ -2449,7 +2452,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="68" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>302</v>
       </c>
@@ -2457,7 +2460,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="69" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>305</v>
       </c>
@@ -2465,7 +2468,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="70" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>308</v>
       </c>
@@ -2473,7 +2476,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="71" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>311</v>
       </c>
@@ -2481,7 +2484,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="72" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>313</v>
       </c>
@@ -2489,7 +2492,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="73" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>315</v>
       </c>
@@ -2497,7 +2500,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="74" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>317</v>
       </c>
@@ -2505,7 +2508,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="75" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>319</v>
       </c>
@@ -2513,7 +2516,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="76" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>321</v>
       </c>
@@ -2521,7 +2524,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="77" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>323</v>
       </c>
@@ -2529,7 +2532,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="78" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>325</v>
       </c>
@@ -2537,7 +2540,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="79" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>327</v>
       </c>
@@ -2545,7 +2548,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="80" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>329</v>
       </c>
@@ -2553,7 +2556,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="81" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>331</v>
       </c>
@@ -2561,7 +2564,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="82" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>333</v>
       </c>
@@ -2569,7 +2572,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="83" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>335</v>
       </c>
@@ -2577,7 +2580,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="84" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>337</v>
       </c>
@@ -2585,7 +2588,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="85" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>339</v>
       </c>
@@ -2593,7 +2596,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="86" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>341</v>
       </c>
@@ -2601,7 +2604,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="87" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>343</v>
       </c>
@@ -2609,7 +2612,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="88" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>345</v>
       </c>
@@ -2617,7 +2620,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="89" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>347</v>
       </c>
@@ -2625,7 +2628,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="90" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>349</v>
       </c>
@@ -2633,7 +2636,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="91" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>351</v>
       </c>
@@ -2641,7 +2644,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="92" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>353</v>
       </c>
@@ -2649,7 +2652,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="93" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>355</v>
       </c>
@@ -2657,7 +2660,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="94" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>357</v>
       </c>
@@ -2665,7 +2668,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="95" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>359</v>
       </c>
@@ -2673,7 +2676,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="96" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>361</v>
       </c>
@@ -2681,7 +2684,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="97" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>363</v>
       </c>
@@ -2689,7 +2692,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="98" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>365</v>
       </c>
@@ -2697,7 +2700,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="99" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>367</v>
       </c>
@@ -2705,7 +2708,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="100" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>369</v>
       </c>
@@ -2713,7 +2716,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="101" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>371</v>
       </c>
@@ -2721,7 +2724,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="102" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>373</v>
       </c>
@@ -2729,7 +2732,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="103" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>375</v>
       </c>
@@ -2737,7 +2740,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="104" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>376</v>
       </c>
@@ -2745,7 +2748,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="105" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>377</v>
       </c>
@@ -2753,7 +2756,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="106" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>378</v>
       </c>
@@ -2761,7 +2764,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="107" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>379</v>
       </c>
@@ -2769,7 +2772,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="108" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>380</v>
       </c>
@@ -2777,7 +2780,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="109" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>381</v>
       </c>
@@ -2785,7 +2788,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="110" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>382</v>
       </c>
@@ -2793,7 +2796,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="111" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>383</v>
       </c>
@@ -2801,7 +2804,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="112" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>471</v>
       </c>
@@ -2809,7 +2812,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="113" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>473</v>
       </c>
@@ -2817,7 +2820,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="114" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>474</v>
       </c>
@@ -2825,7 +2828,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="115" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>475</v>
       </c>
@@ -2833,7 +2836,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="116" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>476</v>
       </c>
@@ -2841,7 +2844,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="117" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>477</v>
       </c>
@@ -2849,7 +2852,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="118" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>478</v>
       </c>
@@ -2857,7 +2860,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="119" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>479</v>
       </c>
@@ -2865,7 +2868,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="120" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>480</v>
       </c>
@@ -2873,7 +2876,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="121" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>481</v>
       </c>
@@ -2881,7 +2884,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="122" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>482</v>
       </c>
@@ -2889,7 +2892,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="123" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>483</v>
       </c>
@@ -2897,7 +2900,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="124" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>85</v>
       </c>
@@ -2905,7 +2908,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="125" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>93</v>
       </c>
@@ -2913,7 +2916,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="126" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>101</v>
       </c>
@@ -2921,7 +2924,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="127" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>107</v>
       </c>
@@ -2929,7 +2932,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="128" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>114</v>
       </c>
@@ -2937,7 +2940,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="129" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>121</v>
       </c>
@@ -2945,7 +2948,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="130" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>128</v>
       </c>
@@ -2953,7 +2956,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="131" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>135</v>
       </c>
@@ -2961,7 +2964,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="132" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>142</v>
       </c>
@@ -2969,7 +2972,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="133" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
         <v>149</v>
       </c>
@@ -2977,7 +2980,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="134" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>156</v>
       </c>
@@ -2985,7 +2988,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="135" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
         <v>163</v>
       </c>
@@ -2993,7 +2996,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="136" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
         <v>170</v>
       </c>
@@ -3001,7 +3004,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="137" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
         <v>175</v>
       </c>
@@ -3009,7 +3012,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="138" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
         <v>180</v>
       </c>
@@ -3017,7 +3020,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="139" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
         <v>185</v>
       </c>
@@ -3025,7 +3028,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="140" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
         <v>190</v>
       </c>
@@ -3033,7 +3036,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="141" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
         <v>195</v>
       </c>
@@ -3041,7 +3044,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="142" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
         <v>200</v>
       </c>
@@ -3049,7 +3052,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="143" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
         <v>205</v>
       </c>
@@ -3057,7 +3060,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="144" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
         <v>210</v>
       </c>
@@ -3065,7 +3068,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="145" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
         <v>215</v>
       </c>
@@ -3073,7 +3076,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="146" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
         <v>220</v>
       </c>
@@ -3081,7 +3084,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="147" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
         <v>225</v>
       </c>
@@ -3089,7 +3092,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="148" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
         <v>230</v>
       </c>
@@ -3097,7 +3100,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="149" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
         <v>235</v>
       </c>
@@ -3105,7 +3108,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="150" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
         <v>240</v>
       </c>
@@ -3113,7 +3116,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="151" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
         <v>245</v>
       </c>
@@ -3121,7 +3124,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="152" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
         <v>250</v>
       </c>
@@ -3129,7 +3132,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="153" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
         <v>254</v>
       </c>
@@ -3137,7 +3140,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="154" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
         <v>258</v>
       </c>
@@ -3145,7 +3148,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="155" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
         <v>262</v>
       </c>
@@ -3153,7 +3156,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="156" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
         <v>266</v>
       </c>
@@ -3161,7 +3164,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="157" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
         <v>270</v>
       </c>
@@ -3169,7 +3172,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="158" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
         <v>274</v>
       </c>
@@ -3177,7 +3180,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="159" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
         <v>278</v>
       </c>
@@ -3185,7 +3188,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="160" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
         <v>282</v>
       </c>
@@ -3193,7 +3196,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="161" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
         <v>285</v>
       </c>
@@ -3201,7 +3204,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="162" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
         <v>288</v>
       </c>
@@ -3209,7 +3212,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="163" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
         <v>291</v>
       </c>
@@ -3217,7 +3220,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="164" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
         <v>294</v>
       </c>
@@ -3225,7 +3228,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="165" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
         <v>297</v>
       </c>
@@ -3233,7 +3236,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="166" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
         <v>300</v>
       </c>
@@ -3241,7 +3244,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="167" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
         <v>303</v>
       </c>
@@ -3249,7 +3252,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="168" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
         <v>306</v>
       </c>
@@ -3257,7 +3260,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="169" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
         <v>309</v>
       </c>
@@ -3265,7 +3268,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="170" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
         <v>312</v>
       </c>
@@ -3273,7 +3276,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="171" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
         <v>314</v>
       </c>
@@ -3281,7 +3284,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="172" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
         <v>316</v>
       </c>
@@ -3289,7 +3292,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="173" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
         <v>318</v>
       </c>
@@ -3297,7 +3300,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="174" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
         <v>320</v>
       </c>
@@ -3305,7 +3308,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="175" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
         <v>322</v>
       </c>
@@ -3313,7 +3316,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="176" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
         <v>324</v>
       </c>
@@ -3321,7 +3324,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="177" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
         <v>326</v>
       </c>
@@ -3329,7 +3332,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="178" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
         <v>328</v>
       </c>
@@ -3337,7 +3340,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="179" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
         <v>330</v>
       </c>
@@ -3345,7 +3348,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="180" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
         <v>332</v>
       </c>
@@ -3353,7 +3356,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="181" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
         <v>334</v>
       </c>
@@ -3361,7 +3364,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="182" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
         <v>336</v>
       </c>
@@ -3369,7 +3372,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="183" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="s">
         <v>338</v>
       </c>
@@ -3377,7 +3380,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="184" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
         <v>340</v>
       </c>
@@ -3385,7 +3388,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="185" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="s">
         <v>342</v>
       </c>
@@ -3393,7 +3396,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="186" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
         <v>344</v>
       </c>
@@ -3401,7 +3404,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="187" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" s="1" t="s">
         <v>346</v>
       </c>
@@ -3409,7 +3412,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="188" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
         <v>348</v>
       </c>
@@ -3417,7 +3420,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="189" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" s="1" t="s">
         <v>350</v>
       </c>
@@ -3425,7 +3428,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="190" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="s">
         <v>352</v>
       </c>
@@ -3433,7 +3436,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="191" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" s="1" t="s">
         <v>354</v>
       </c>
@@ -3441,7 +3444,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="192" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
         <v>356</v>
       </c>
@@ -3449,7 +3452,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="193" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
         <v>358</v>
       </c>
@@ -3457,7 +3460,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="194" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
         <v>360</v>
       </c>
@@ -3465,7 +3468,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="195" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" s="1" t="s">
         <v>362</v>
       </c>
@@ -3473,7 +3476,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="196" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
         <v>364</v>
       </c>
@@ -3481,7 +3484,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="197" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" s="1" t="s">
         <v>366</v>
       </c>
@@ -3489,7 +3492,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="198" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" s="1" t="s">
         <v>368</v>
       </c>
@@ -3497,7 +3500,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="199" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" s="1" t="s">
         <v>370</v>
       </c>
@@ -3505,7 +3508,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="200" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" s="1" t="s">
         <v>372</v>
       </c>
@@ -3513,7 +3516,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="201" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" s="1" t="s">
         <v>374</v>
       </c>
@@ -3905,7 +3908,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="250" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A250" s="1" t="s">
         <v>2</v>
       </c>
@@ -3913,7 +3916,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="251" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A251" s="1" t="s">
         <v>9</v>
       </c>
@@ -3921,7 +3924,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="252" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A252" s="1" t="s">
         <v>16</v>
       </c>
@@ -3929,7 +3932,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="253" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A253" s="1" t="s">
         <v>23</v>
       </c>
@@ -3937,7 +3940,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="254" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A254" s="1" t="s">
         <v>30</v>
       </c>
@@ -3945,7 +3948,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="255" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A255" s="1" t="s">
         <v>37</v>
       </c>
@@ -3953,7 +3956,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="256" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A256" s="1" t="s">
         <v>44</v>
       </c>
@@ -3961,7 +3964,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="257" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A257" s="1" t="s">
         <v>51</v>
       </c>
@@ -3969,7 +3972,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="258" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A258" s="1" t="s">
         <v>58</v>
       </c>
@@ -3977,7 +3980,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="259" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A259" s="1" t="s">
         <v>65</v>
       </c>
@@ -3985,7 +3988,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="260" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A260" s="1" t="s">
         <v>72</v>
       </c>
@@ -3993,7 +3996,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="261" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A261" s="1" t="s">
         <v>79</v>
       </c>
@@ -4001,7 +4004,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="262" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A262" s="1" t="s">
         <v>87</v>
       </c>
@@ -4009,7 +4012,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="263" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A263" s="1" t="s">
         <v>95</v>
       </c>
@@ -4017,7 +4020,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="264" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A264" s="1" t="s">
         <v>103</v>
       </c>
@@ -4025,7 +4028,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="265" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A265" s="1" t="s">
         <v>109</v>
       </c>
@@ -4033,7 +4036,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="266" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A266" s="1" t="s">
         <v>116</v>
       </c>
@@ -4041,7 +4044,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="267" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A267" s="1" t="s">
         <v>123</v>
       </c>
@@ -4049,7 +4052,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="268" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A268" s="1" t="s">
         <v>130</v>
       </c>
@@ -4057,7 +4060,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="269" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A269" s="1" t="s">
         <v>137</v>
       </c>
@@ -4065,7 +4068,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="270" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A270" s="1" t="s">
         <v>144</v>
       </c>
@@ -4073,7 +4076,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="271" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A271" s="1" t="s">
         <v>151</v>
       </c>
@@ -4081,7 +4084,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="272" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A272" s="1" t="s">
         <v>158</v>
       </c>
@@ -4089,7 +4092,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="273" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A273" s="1" t="s">
         <v>165</v>
       </c>
@@ -4097,7 +4100,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="274" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A274" s="1" t="s">
         <v>172</v>
       </c>
@@ -4105,7 +4108,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="275" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A275" s="1" t="s">
         <v>177</v>
       </c>
@@ -4113,7 +4116,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="276" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A276" s="1" t="s">
         <v>182</v>
       </c>
@@ -4121,7 +4124,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="277" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A277" s="1" t="s">
         <v>187</v>
       </c>
@@ -4129,7 +4132,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="278" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A278" s="1" t="s">
         <v>192</v>
       </c>
@@ -4137,7 +4140,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="279" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A279" s="1" t="s">
         <v>197</v>
       </c>
@@ -4145,7 +4148,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="280" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A280" s="1" t="s">
         <v>202</v>
       </c>
@@ -4153,7 +4156,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="281" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A281" s="1" t="s">
         <v>207</v>
       </c>
@@ -4161,7 +4164,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="282" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A282" s="1" t="s">
         <v>212</v>
       </c>
@@ -4169,7 +4172,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="283" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A283" s="1" t="s">
         <v>217</v>
       </c>
@@ -4177,7 +4180,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="284" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A284" s="1" t="s">
         <v>222</v>
       </c>
@@ -4185,7 +4188,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="285" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A285" s="1" t="s">
         <v>227</v>
       </c>
@@ -4193,7 +4196,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="286" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A286" s="1" t="s">
         <v>232</v>
       </c>
@@ -4201,7 +4204,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="287" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A287" s="1" t="s">
         <v>237</v>
       </c>
@@ -4209,7 +4212,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="288" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A288" s="1" t="s">
         <v>242</v>
       </c>
@@ -4217,7 +4220,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="289" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A289" s="1" t="s">
         <v>247</v>
       </c>
@@ -4225,7 +4228,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="290" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A290" s="1" t="s">
         <v>252</v>
       </c>
@@ -4233,7 +4236,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="291" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A291" s="1" t="s">
         <v>256</v>
       </c>
@@ -4241,7 +4244,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="292" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A292" s="1" t="s">
         <v>260</v>
       </c>
@@ -4249,7 +4252,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="293" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A293" s="1" t="s">
         <v>264</v>
       </c>
@@ -4257,7 +4260,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="294" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A294" s="1" t="s">
         <v>268</v>
       </c>
@@ -4265,7 +4268,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="295" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A295" s="1" t="s">
         <v>272</v>
       </c>
@@ -4273,7 +4276,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="296" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A296" s="1" t="s">
         <v>276</v>
       </c>
@@ -4281,7 +4284,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="297" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A297" s="1" t="s">
         <v>280</v>
       </c>
@@ -4289,7 +4292,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="298" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A298" s="1" t="s">
         <v>4</v>
       </c>
@@ -4297,7 +4300,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="299" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A299" s="1" t="s">
         <v>11</v>
       </c>
@@ -4305,7 +4308,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="300" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A300" s="1" t="s">
         <v>18</v>
       </c>
@@ -4313,7 +4316,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="301" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A301" s="1" t="s">
         <v>25</v>
       </c>
@@ -4321,7 +4324,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="302" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A302" s="1" t="s">
         <v>32</v>
       </c>
@@ -4329,7 +4332,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="303" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A303" s="1" t="s">
         <v>39</v>
       </c>
@@ -4337,7 +4340,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="304" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A304" s="1" t="s">
         <v>46</v>
       </c>
@@ -4345,7 +4348,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="305" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A305" s="1" t="s">
         <v>53</v>
       </c>
@@ -4353,7 +4356,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="306" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A306" s="1" t="s">
         <v>60</v>
       </c>
@@ -4361,7 +4364,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="307" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A307" s="1" t="s">
         <v>67</v>
       </c>
@@ -4369,7 +4372,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="308" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A308" s="1" t="s">
         <v>74</v>
       </c>
@@ -4377,7 +4380,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="309" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A309" s="1" t="s">
         <v>81</v>
       </c>
@@ -4385,7 +4388,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="310" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A310" s="1" t="s">
         <v>89</v>
       </c>
@@ -4393,7 +4396,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="311" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A311" s="1" t="s">
         <v>97</v>
       </c>
@@ -4401,7 +4404,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="312" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A312" s="1" t="s">
         <v>97</v>
       </c>
@@ -4409,489 +4412,489 @@
         <v>484</v>
       </c>
     </row>
-    <row r="313" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A313" s="1" t="s">
-        <v>111</v>
+        <v>493</v>
       </c>
       <c r="B313" s="2" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="314" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A314" s="1" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="B314" s="2" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="315" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A315" s="1" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="B315" s="2" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="316" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A316" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B316" s="2" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="317" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A317" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="B316" s="2" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="317" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A317" s="1" t="s">
-        <v>139</v>
       </c>
       <c r="B317" s="2" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="318" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A318" s="1" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="B318" s="2" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="319" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A319" s="1" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="B319" s="2" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="320" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A320" s="1" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="B320" s="2" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="321" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A321" s="1" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="B321" s="2" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="322" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A322" s="1" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="B322" s="2" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="323" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A323" s="1" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="B323" s="2" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="324" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A324" s="1" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="B324" s="2" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="325" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A325" s="1" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="B325" s="2" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="326" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A326" s="1" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="B326" s="2" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="327" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A327" s="1" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="B327" s="2" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="328" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A328" s="1" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="B328" s="2" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="329" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A329" s="1" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="B329" s="2" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="330" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A330" s="1" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="B330" s="2" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="331" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A331" s="1" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="B331" s="2" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="332" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A332" s="1" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="B332" s="2" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="333" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A333" s="1" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="B333" s="2" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="334" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A334" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B334" s="2" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="335" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A335" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B334" s="1" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="335" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A335" s="1" t="s">
+      <c r="B335" s="1" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="336" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A336" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B335" s="1" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="336" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A336" s="1" t="s">
+      <c r="B336" s="1" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="337" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A337" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B336" s="1" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="337" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A337" s="1" t="s">
+      <c r="B337" s="1" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="338" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A338" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B337" s="1" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="338" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A338" s="1" t="s">
+      <c r="B338" s="1" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="339" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A339" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B338" s="1" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="339" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A339" s="1" t="s">
+      <c r="B339" s="1" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="340" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A340" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B339" s="1" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="340" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A340" s="1" t="s">
+      <c r="B340" s="1" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="341" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A341" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B340" s="1" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="341" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A341" s="1" t="s">
+      <c r="B341" s="1" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="342" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A342" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B341" s="1" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="342" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A342" s="1" t="s">
+      <c r="B342" s="1" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="343" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A343" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B342" s="1" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="343" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A343" s="1" t="s">
+      <c r="B343" s="1" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="344" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A344" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B343" s="1" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="344" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A344" s="1" t="s">
+      <c r="B344" s="1" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="345" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A345" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B344" s="1" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="345" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A345" s="1" t="s">
+      <c r="B345" s="1" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="346" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A346" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B345" s="1" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="346" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A346" s="1" t="s">
+      <c r="B346" s="1" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="347" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A347" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B346" s="1" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="347" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A347" s="1" t="s">
+      <c r="B347" s="1" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="348" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A348" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B347" s="1" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="348" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A348" s="1" t="s">
+      <c r="B348" s="1" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="349" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A349" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B348" s="1" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="349" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A349" s="1" t="s">
+      <c r="B349" s="1" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="350" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A350" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B349" s="1" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="350" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A350" s="1" t="s">
+      <c r="B350" s="1" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="351" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A351" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B350" s="1" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="351" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A351" s="1" t="s">
+      <c r="B351" s="1" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="352" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A352" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B351" s="1" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="352" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A352" s="1" t="s">
+      <c r="B352" s="1" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="353" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A353" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B352" s="1" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="353" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A353" s="1" t="s">
+      <c r="B353" s="1" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="354" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A354" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B353" s="1" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="354" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A354" s="1" t="s">
+      <c r="B354" s="1" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="355" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A355" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B354" s="1" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="355" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A355" s="1" t="s">
+      <c r="B355" s="1" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="356" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A356" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="B355" s="1" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="356" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A356" s="1" t="s">
+      <c r="B356" s="1" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="357" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A357" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="B356" s="1" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="357" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A357" s="1" t="s">
+      <c r="B357" s="1" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="358" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A358" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B357" s="1" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="358" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A358" s="1" t="s">
+      <c r="B358" s="1" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="359" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A359" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="B358" s="1" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="359" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A359" s="1" t="s">
+      <c r="B359" s="1" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="360" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A360" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="B359" s="1" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="360" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A360" s="1" t="s">
+      <c r="B360" s="1" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="361" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A361" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="B360" s="1" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="361" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A361" s="1" t="s">
+      <c r="B361" s="1" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="362" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A362" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="B361" s="1" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="362" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A362" s="1" t="s">
+      <c r="B362" s="1" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="363" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A363" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B362" s="1" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="363" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A363" s="1" t="s">
+      <c r="B363" s="1" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="364" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A364" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="B363" s="1" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="364" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A364" s="1" t="s">
+      <c r="B364" s="1" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="365" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A365" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="B364" s="1" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="365" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A365" s="1" t="s">
+      <c r="B365" s="1" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="366" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A366" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="B365" s="1" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="366" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A366" s="1" t="s">
+      <c r="B366" s="1" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="367" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A367" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="B366" s="1" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="367" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A367" s="1" t="s">
+      <c r="B367" s="1" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="368" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A368" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="B367" s="1" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="368" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A368" s="1" t="s">
+      <c r="B368" s="1" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="369" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A369" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="B368" s="1" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="369" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A369" s="1" t="s">
+      <c r="B369" s="1" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="370" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A370" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="B369" s="1" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="370" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A370" s="1" t="s">
+      <c r="B370" s="1" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="371" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A371" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="B370" s="1" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="371" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A371" s="1" t="s">
+      <c r="B371" s="1" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="372" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A372" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="B371" s="1" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="372" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A372" s="1" t="s">
+      <c r="B372" s="1" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="373" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A373" s="1" t="s">
         <v>243</v>
-      </c>
-      <c r="B372" s="1" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="373" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A373" s="1" t="s">
-        <v>248</v>
       </c>
       <c r="B373" s="1" t="s">
         <v>491</v>
@@ -4899,15 +4902,15 @@
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A374" s="1" t="s">
-        <v>86</v>
+        <v>248</v>
       </c>
       <c r="B374" s="1" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="375" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A375" s="1" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="B375" s="1" t="s">
         <v>492</v>
@@ -4915,7 +4918,7 @@
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A376" s="1" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B376" s="1" t="s">
         <v>492</v>
@@ -4923,7 +4926,7 @@
     </row>
     <row r="377" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A377" s="1" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B377" s="1" t="s">
         <v>492</v>
@@ -4931,7 +4934,7 @@
     </row>
     <row r="378" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A378" s="1" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="B378" s="1" t="s">
         <v>492</v>
@@ -4939,7 +4942,7 @@
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A379" s="1" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="B379" s="1" t="s">
         <v>492</v>
@@ -4947,7 +4950,7 @@
     </row>
     <row r="380" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A380" s="1" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="B380" s="1" t="s">
         <v>492</v>
@@ -4955,7 +4958,7 @@
     </row>
     <row r="381" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A381" s="1" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="B381" s="1" t="s">
         <v>492</v>
@@ -4963,7 +4966,7 @@
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A382" s="1" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="B382" s="1" t="s">
         <v>492</v>
@@ -4971,295 +4974,295 @@
     </row>
     <row r="383" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A383" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B383" s="1" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="384" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A384" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B383" s="1" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="384" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A384" s="1" t="s">
+      <c r="B384" s="1" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="385" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A385" s="1" t="s">
         <v>384</v>
-      </c>
-      <c r="B384" s="2" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="385" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A385" s="1" t="s">
-        <v>385</v>
       </c>
       <c r="B385" s="2" t="s">
         <v>486</v>
       </c>
     </row>
-    <row r="386" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A386" s="1" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B386" s="2" t="s">
         <v>486</v>
       </c>
     </row>
-    <row r="387" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A387" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B387" s="2" t="s">
         <v>486</v>
       </c>
     </row>
-    <row r="388" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A388" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B388" s="2" t="s">
         <v>486</v>
       </c>
     </row>
-    <row r="389" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A389" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B389" s="2" t="s">
         <v>486</v>
       </c>
     </row>
-    <row r="390" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A390" s="1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B390" s="2" t="s">
         <v>486</v>
       </c>
     </row>
-    <row r="391" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A391" s="1" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B391" s="2" t="s">
         <v>486</v>
       </c>
     </row>
-    <row r="392" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A392" s="1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B392" s="2" t="s">
         <v>486</v>
       </c>
     </row>
-    <row r="393" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A393" s="1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B393" s="2" t="s">
         <v>486</v>
       </c>
     </row>
-    <row r="394" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A394" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B394" s="2" t="s">
         <v>486</v>
       </c>
     </row>
-    <row r="395" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A395" s="1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B395" s="2" t="s">
         <v>486</v>
       </c>
     </row>
-    <row r="396" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A396" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="B396" s="2" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="397" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A397" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B396" s="1" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="397" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A397" s="1" t="s">
+      <c r="B397" s="1" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="398" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A398" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B397" s="1" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="398" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A398" s="1" t="s">
+      <c r="B398" s="1" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="399" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A399" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B398" s="1" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="399" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A399" s="1" t="s">
+      <c r="B399" s="1" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="400" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A400" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B399" s="1" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="400" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A400" s="1" t="s">
+      <c r="B400" s="1" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="401" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A401" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B400" s="1" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="401" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A401" s="1" t="s">
+      <c r="B401" s="1" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="402" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A402" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B401" s="1" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="402" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A402" s="1" t="s">
+      <c r="B402" s="1" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="403" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A403" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B402" s="1" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="403" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A403" s="1" t="s">
+      <c r="B403" s="1" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="404" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A404" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B403" s="1" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="404" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A404" s="1" t="s">
+      <c r="B404" s="1" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="405" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A405" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B404" s="1" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="405" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A405" s="1" t="s">
+      <c r="B405" s="1" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="406" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A406" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B405" s="1" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="406" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A406" s="1" t="s">
+      <c r="B406" s="1" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="407" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A407" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B406" s="1" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="407" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A407" s="1" t="s">
+      <c r="B407" s="1" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="408" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A408" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B407" s="1" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="408" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A408" s="1" t="s">
+      <c r="B408" s="1" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="409" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A409" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B408" s="1" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="409" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A409" s="1" t="s">
+      <c r="B409" s="1" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="410" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A410" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B409" s="1" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="410" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A410" s="1" t="s">
+      <c r="B410" s="1" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="411" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A411" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B410" s="1" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="411" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A411" s="1" t="s">
+      <c r="B411" s="1" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="412" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A412" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B411" s="1" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="412" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A412" s="1" t="s">
+      <c r="B412" s="1" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="413" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A413" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B412" s="1" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="413" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A413" s="1" t="s">
+      <c r="B413" s="1" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="414" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A414" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B413" s="1" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="414" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A414" s="1" t="s">
+      <c r="B414" s="1" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="415" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A415" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B414" s="1" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="415" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A415" s="1" t="s">
+      <c r="B415" s="1" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="416" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A416" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B415" s="1" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="416" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A416" s="1" t="s">
+      <c r="B416" s="1" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="417" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A417" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="B416" s="1" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="417" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A417" s="1" t="s">
+      <c r="B417" s="1" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="418" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A418" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="B417" s="1" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="418" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A418" s="1" t="s">
+      <c r="B418" s="1" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="419" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A419" s="1" t="s">
         <v>161</v>
-      </c>
-      <c r="B418" s="1" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="419" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A419" s="1" t="s">
-        <v>168</v>
       </c>
       <c r="B419" s="1" t="s">
         <v>490</v>
@@ -5267,15 +5270,15 @@
     </row>
     <row r="420" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A420" s="1" t="s">
-        <v>6</v>
+        <v>168</v>
       </c>
       <c r="B420" s="1" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="421" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A421" s="1" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B421" s="1" t="s">
         <v>492</v>
@@ -5283,7 +5286,7 @@
     </row>
     <row r="422" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A422" s="1" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B422" s="1" t="s">
         <v>492</v>
@@ -5291,7 +5294,7 @@
     </row>
     <row r="423" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A423" s="1" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B423" s="1" t="s">
         <v>492</v>
@@ -5299,7 +5302,7 @@
     </row>
     <row r="424" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A424" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B424" s="1" t="s">
         <v>492</v>
@@ -5307,7 +5310,7 @@
     </row>
     <row r="425" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A425" s="1" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B425" s="1" t="s">
         <v>492</v>
@@ -5315,7 +5318,7 @@
     </row>
     <row r="426" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A426" s="1" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B426" s="1" t="s">
         <v>492</v>
@@ -5323,7 +5326,7 @@
     </row>
     <row r="427" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A427" s="1" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B427" s="1" t="s">
         <v>492</v>
@@ -5331,7 +5334,7 @@
     </row>
     <row r="428" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A428" s="1" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="B428" s="1" t="s">
         <v>492</v>
@@ -5339,7 +5342,7 @@
     </row>
     <row r="429" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A429" s="1" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="B429" s="1" t="s">
         <v>492</v>
@@ -5347,7 +5350,7 @@
     </row>
     <row r="430" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A430" s="1" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="B430" s="1" t="s">
         <v>492</v>
@@ -5355,7 +5358,7 @@
     </row>
     <row r="431" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A431" s="1" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="B431" s="1" t="s">
         <v>492</v>
@@ -5363,7 +5366,7 @@
     </row>
     <row r="432" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A432" s="1" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="B432" s="1" t="s">
         <v>492</v>
@@ -5371,412 +5374,414 @@
     </row>
     <row r="433" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A433" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B433" s="1" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="434" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A434" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B433" s="1" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="434" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A434" s="3" t="s">
+      <c r="B434" s="1" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="435" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A435" s="3" t="s">
         <v>414</v>
-      </c>
-      <c r="B434" s="1" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="435" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A435" s="3" t="s">
-        <v>415</v>
       </c>
       <c r="B435" s="1" t="s">
         <v>488</v>
       </c>
     </row>
-    <row r="436" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A436" s="3" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B436" s="1" t="s">
         <v>488</v>
       </c>
     </row>
-    <row r="437" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A437" s="3" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B437" s="1" t="s">
         <v>488</v>
       </c>
     </row>
-    <row r="438" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A438" s="3" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B438" s="1" t="s">
         <v>488</v>
       </c>
     </row>
-    <row r="439" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A439" s="3" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B439" s="1" t="s">
         <v>488</v>
       </c>
     </row>
-    <row r="440" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A440" s="3" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B440" s="1" t="s">
         <v>488</v>
       </c>
     </row>
-    <row r="441" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A441" s="3" t="s">
+        <v>420</v>
+      </c>
+      <c r="B441" s="1" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="442" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A442" s="3" t="s">
         <v>421</v>
-      </c>
-      <c r="B441" s="1" t="s">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="442" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A442" s="3" t="s">
-        <v>422</v>
       </c>
       <c r="B442" s="1" t="s">
         <v>489</v>
       </c>
     </row>
-    <row r="443" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A443" s="3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B443" s="1" t="s">
         <v>489</v>
       </c>
     </row>
-    <row r="444" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A444" s="3" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B444" s="1" t="s">
         <v>489</v>
       </c>
     </row>
-    <row r="445" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A445" s="3" t="s">
+        <v>424</v>
+      </c>
+      <c r="B445" s="1" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="446" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A446" s="3" t="s">
         <v>425</v>
-      </c>
-      <c r="B445" s="1" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="446" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A446" s="3" t="s">
-        <v>426</v>
       </c>
       <c r="B446" s="1" t="s">
         <v>488</v>
       </c>
     </row>
-    <row r="447" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A447" s="3" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B447" s="1" t="s">
         <v>488</v>
       </c>
     </row>
-    <row r="448" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A448" s="3" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B448" s="1" t="s">
         <v>488</v>
       </c>
     </row>
-    <row r="449" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A449" s="3" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B449" s="1" t="s">
         <v>488</v>
       </c>
     </row>
-    <row r="450" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A450" s="3" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B450" s="1" t="s">
         <v>488</v>
       </c>
     </row>
-    <row r="451" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A451" s="3" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B451" s="1" t="s">
         <v>488</v>
       </c>
     </row>
-    <row r="452" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A452" s="3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B452" s="1" t="s">
         <v>488</v>
       </c>
     </row>
-    <row r="453" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A453" s="3" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B453" s="1" t="s">
         <v>488</v>
       </c>
     </row>
-    <row r="454" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A454" s="3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B454" s="1" t="s">
         <v>488</v>
       </c>
     </row>
-    <row r="455" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A455" s="3" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B455" s="1" t="s">
         <v>488</v>
       </c>
     </row>
-    <row r="456" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A456" s="3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B456" s="1" t="s">
         <v>488</v>
       </c>
     </row>
-    <row r="457" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A457" s="3" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B457" s="1" t="s">
         <v>488</v>
       </c>
     </row>
-    <row r="458" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A458" s="3" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B458" s="1" t="s">
         <v>488</v>
       </c>
     </row>
-    <row r="459" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A459" s="3" t="s">
+        <v>438</v>
+      </c>
+      <c r="B459" s="1" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="460" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A460" s="3" t="s">
         <v>439</v>
-      </c>
-      <c r="B459" s="1" t="s">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="460" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A460" s="3" t="s">
-        <v>440</v>
       </c>
       <c r="B460" s="1" t="s">
         <v>489</v>
       </c>
     </row>
-    <row r="461" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A461" s="3" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B461" s="1" t="s">
         <v>489</v>
       </c>
     </row>
-    <row r="462" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A462" s="3" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B462" s="1" t="s">
         <v>489</v>
       </c>
     </row>
-    <row r="463" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A463" s="3" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B463" s="1" t="s">
         <v>489</v>
       </c>
     </row>
-    <row r="464" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A464" s="3" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B464" s="1" t="s">
         <v>489</v>
       </c>
     </row>
-    <row r="465" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A465" s="3" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B465" s="1" t="s">
         <v>489</v>
       </c>
     </row>
-    <row r="466" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="466" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A466" s="3" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B466" s="1" t="s">
         <v>489</v>
       </c>
     </row>
-    <row r="467" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="467" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A467" s="3" t="s">
+        <v>446</v>
+      </c>
+      <c r="B467" s="1" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="468" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A468" s="3" t="s">
         <v>398</v>
-      </c>
-      <c r="B467" s="1" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="468" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A468" s="3" t="s">
-        <v>399</v>
       </c>
       <c r="B468" s="1" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="469" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="469" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A469" s="3" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B469" s="1" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="470" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="470" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A470" s="3" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B470" s="1" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="471" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="471" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A471" s="3" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B471" s="1" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="472" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="472" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A472" s="3" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B472" s="1" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="473" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="473" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A473" s="3" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B473" s="1" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="474" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="474" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A474" s="3" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B474" s="1" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="475" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="475" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A475" s="3" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B475" s="1" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="476" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="476" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A476" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B476" s="1" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="477" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="477" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A477" s="3" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B477" s="1" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="478" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="478" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A478" s="3" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B478" s="1" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="479" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="479" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A479" s="3" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B479" s="1" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="480" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="480" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A480" s="3" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B480" s="1" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="481" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="481" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A481" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B481" s="1" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="482" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="482" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A482" s="3" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B482" s="1" t="s">
         <v>397</v>
       </c>
     </row>
+    <row r="483" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A483" s="3" t="s">
+        <v>413</v>
+      </c>
+      <c r="B483" s="1" t="s">
+        <v>397</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:B482" xr:uid="{E3722E28-546D-45F9-BF38-B4D5FA1D8738}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="apanha_bc"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:B483" xr:uid="{E3722E28-546D-45F9-BF38-B4D5FA1D8738}"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
realocando parte do local de apanha b para local de alimento
</commit_message>
<xml_diff>
--- a/data/analise_curva_abc/local/datasets/local_apanha_cx.xlsx
+++ b/data/analise_curva_abc/local/datasets/local_apanha_cx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://maxifarmabr-my.sharepoint.com/personal/controle_estoque_grupomaxifarma_com_br/Documents/Documentos/estoque.renan/projetos/projeto_curva_abc/data/analise_curva_abc/local/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="67" documentId="13_ncr:1_{62563889-610E-48F9-917B-CDA4FE3D6C5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C63CE5A0-1111-4EE1-BF1A-15737A227B52}"/>
+  <xr:revisionPtr revIDLastSave="73" documentId="13_ncr:1_{62563889-610E-48F9-917B-CDA4FE3D6C5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FC5E2E46-8D33-4EB4-BD07-0C29DCBD3978}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{18EFAD8D-C71D-455A-9E0F-2475F39BFCF9}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="964" uniqueCount="494">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="964" uniqueCount="495">
   <si>
     <t>local</t>
   </si>
@@ -1510,6 +1510,9 @@
   </si>
   <si>
     <t>010-042-01-01</t>
+  </si>
+  <si>
+    <t>alimento</t>
   </si>
 </sst>
 </file>
@@ -1903,11 +1906,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3722E28-546D-45F9-BF38-B4D5FA1D8738}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:D482"/>
+  <dimension ref="A1:F482"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A250" sqref="A250:A373"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1916,7 +1918,7 @@
     <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>396</v>
       </c>
@@ -1924,7 +1926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -1932,7 +1934,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="3" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -1940,7 +1942,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="4" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
@@ -1948,7 +1950,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="5" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>28</v>
       </c>
@@ -1956,7 +1958,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="6" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>35</v>
       </c>
@@ -1964,7 +1966,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="7" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>42</v>
       </c>
@@ -1972,7 +1974,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="8" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>49</v>
       </c>
@@ -1980,15 +1982,16 @@
         <v>490</v>
       </c>
     </row>
-    <row r="9" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>56</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>490</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F9" s="4"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>63</v>
       </c>
@@ -1997,7 +2000,7 @@
       </c>
       <c r="D10" s="4"/>
     </row>
-    <row r="11" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>70</v>
       </c>
@@ -2005,7 +2008,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="12" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>77</v>
       </c>
@@ -2013,7 +2016,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="13" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>84</v>
       </c>
@@ -2021,7 +2024,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="14" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>92</v>
       </c>
@@ -2029,7 +2032,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="15" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>100</v>
       </c>
@@ -2037,7 +2040,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="16" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>106</v>
       </c>
@@ -2045,7 +2048,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="17" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>113</v>
       </c>
@@ -2053,7 +2056,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="18" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>120</v>
       </c>
@@ -2061,7 +2064,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="19" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>127</v>
       </c>
@@ -2069,7 +2072,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="20" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>134</v>
       </c>
@@ -2077,7 +2080,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="21" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>141</v>
       </c>
@@ -2085,7 +2088,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="22" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>148</v>
       </c>
@@ -2093,7 +2096,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="23" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>155</v>
       </c>
@@ -2101,7 +2104,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="24" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>162</v>
       </c>
@@ -2109,7 +2112,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="25" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>169</v>
       </c>
@@ -2117,7 +2120,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="26" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>447</v>
       </c>
@@ -2125,7 +2128,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="27" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>448</v>
       </c>
@@ -2133,7 +2136,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="28" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>449</v>
       </c>
@@ -2141,7 +2144,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="29" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>450</v>
       </c>
@@ -2149,7 +2152,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="30" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>451</v>
       </c>
@@ -2157,7 +2160,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="31" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>452</v>
       </c>
@@ -2165,7 +2168,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="32" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>453</v>
       </c>
@@ -2173,7 +2176,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="33" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>454</v>
       </c>
@@ -2181,7 +2184,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="34" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>455</v>
       </c>
@@ -2189,7 +2192,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="35" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>456</v>
       </c>
@@ -2197,7 +2200,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="36" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>457</v>
       </c>
@@ -2205,7 +2208,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="37" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>458</v>
       </c>
@@ -2213,7 +2216,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="38" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>459</v>
       </c>
@@ -2221,7 +2224,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="39" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>460</v>
       </c>
@@ -2229,7 +2232,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="40" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>461</v>
       </c>
@@ -2237,7 +2240,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="41" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>462</v>
       </c>
@@ -2245,7 +2248,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="42" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>463</v>
       </c>
@@ -2253,7 +2256,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="43" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>464</v>
       </c>
@@ -2261,7 +2264,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="44" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>465</v>
       </c>
@@ -2269,7 +2272,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="45" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>466</v>
       </c>
@@ -2277,7 +2280,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="46" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>467</v>
       </c>
@@ -2285,7 +2288,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="47" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>468</v>
       </c>
@@ -2293,7 +2296,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="48" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>469</v>
       </c>
@@ -2301,7 +2304,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="49" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>470</v>
       </c>
@@ -2309,7 +2312,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="50" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>234</v>
       </c>
@@ -2317,7 +2320,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="51" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>239</v>
       </c>
@@ -2325,7 +2328,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="52" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>244</v>
       </c>
@@ -2333,7 +2336,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="53" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>249</v>
       </c>
@@ -2341,7 +2344,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="54" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>253</v>
       </c>
@@ -2349,7 +2352,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="55" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>257</v>
       </c>
@@ -2357,7 +2360,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="56" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>261</v>
       </c>
@@ -2365,7 +2368,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="57" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>265</v>
       </c>
@@ -2373,7 +2376,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="58" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>269</v>
       </c>
@@ -2381,7 +2384,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="59" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>273</v>
       </c>
@@ -2389,7 +2392,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="60" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>277</v>
       </c>
@@ -2397,7 +2400,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="61" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>281</v>
       </c>
@@ -2405,7 +2408,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="62" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>284</v>
       </c>
@@ -2413,7 +2416,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="63" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>287</v>
       </c>
@@ -2421,7 +2424,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="64" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>290</v>
       </c>
@@ -2429,7 +2432,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="65" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>293</v>
       </c>
@@ -2437,7 +2440,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="66" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>296</v>
       </c>
@@ -2445,7 +2448,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="67" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>299</v>
       </c>
@@ -2453,7 +2456,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="68" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>302</v>
       </c>
@@ -2461,7 +2464,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="69" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>305</v>
       </c>
@@ -2469,7 +2472,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="70" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>308</v>
       </c>
@@ -2477,7 +2480,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="71" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>311</v>
       </c>
@@ -2485,7 +2488,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="72" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>313</v>
       </c>
@@ -2493,7 +2496,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="73" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>315</v>
       </c>
@@ -2501,7 +2504,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="74" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>317</v>
       </c>
@@ -2509,7 +2512,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="75" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>319</v>
       </c>
@@ -2517,7 +2520,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="76" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>321</v>
       </c>
@@ -2525,7 +2528,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="77" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>323</v>
       </c>
@@ -2533,7 +2536,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="78" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>325</v>
       </c>
@@ -2541,7 +2544,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="79" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>327</v>
       </c>
@@ -2549,7 +2552,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="80" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>329</v>
       </c>
@@ -2557,7 +2560,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="81" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>331</v>
       </c>
@@ -2565,7 +2568,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="82" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>333</v>
       </c>
@@ -2573,7 +2576,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="83" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>335</v>
       </c>
@@ -2581,7 +2584,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="84" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>337</v>
       </c>
@@ -2589,7 +2592,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="85" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>339</v>
       </c>
@@ -2597,7 +2600,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="86" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>341</v>
       </c>
@@ -2605,7 +2608,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="87" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>343</v>
       </c>
@@ -2613,7 +2616,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="88" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>345</v>
       </c>
@@ -2621,7 +2624,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="89" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>347</v>
       </c>
@@ -2629,7 +2632,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="90" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>349</v>
       </c>
@@ -2637,7 +2640,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="91" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>351</v>
       </c>
@@ -2645,7 +2648,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="92" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>353</v>
       </c>
@@ -2653,7 +2656,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="93" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>355</v>
       </c>
@@ -2661,7 +2664,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="94" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>357</v>
       </c>
@@ -2669,7 +2672,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="95" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>359</v>
       </c>
@@ -2677,7 +2680,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="96" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>361</v>
       </c>
@@ -2685,7 +2688,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="97" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>363</v>
       </c>
@@ -2693,7 +2696,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="98" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>365</v>
       </c>
@@ -2701,7 +2704,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="99" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>367</v>
       </c>
@@ -2709,7 +2712,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="100" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>369</v>
       </c>
@@ -2717,7 +2720,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="101" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>371</v>
       </c>
@@ -2725,7 +2728,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="102" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>373</v>
       </c>
@@ -2733,7 +2736,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="103" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>375</v>
       </c>
@@ -2741,7 +2744,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="104" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>376</v>
       </c>
@@ -2749,7 +2752,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="105" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>377</v>
       </c>
@@ -2757,7 +2760,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="106" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>378</v>
       </c>
@@ -2765,7 +2768,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="107" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>379</v>
       </c>
@@ -2773,7 +2776,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="108" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>380</v>
       </c>
@@ -2781,7 +2784,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="109" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>381</v>
       </c>
@@ -2789,7 +2792,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="110" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>382</v>
       </c>
@@ -2797,7 +2800,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="111" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>383</v>
       </c>
@@ -2805,7 +2808,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="112" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>471</v>
       </c>
@@ -2813,7 +2816,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="113" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>473</v>
       </c>
@@ -2821,7 +2824,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="114" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>474</v>
       </c>
@@ -2829,7 +2832,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="115" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>475</v>
       </c>
@@ -2837,7 +2840,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="116" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>476</v>
       </c>
@@ -2845,7 +2848,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="117" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>477</v>
       </c>
@@ -2853,7 +2856,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="118" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>478</v>
       </c>
@@ -2861,7 +2864,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="119" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>479</v>
       </c>
@@ -2869,7 +2872,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="120" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>480</v>
       </c>
@@ -2877,7 +2880,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="121" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>481</v>
       </c>
@@ -2885,7 +2888,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="122" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>482</v>
       </c>
@@ -2893,7 +2896,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="123" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>483</v>
       </c>
@@ -2901,7 +2904,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="124" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>85</v>
       </c>
@@ -2909,7 +2912,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="125" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>93</v>
       </c>
@@ -2917,7 +2920,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="126" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>101</v>
       </c>
@@ -2925,7 +2928,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="127" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>107</v>
       </c>
@@ -2933,7 +2936,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="128" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>114</v>
       </c>
@@ -2941,7 +2944,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="129" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>121</v>
       </c>
@@ -2949,7 +2952,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="130" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>128</v>
       </c>
@@ -2957,7 +2960,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="131" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>135</v>
       </c>
@@ -2965,7 +2968,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="132" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>142</v>
       </c>
@@ -2973,7 +2976,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="133" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
         <v>149</v>
       </c>
@@ -2981,7 +2984,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="134" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>156</v>
       </c>
@@ -2989,7 +2992,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="135" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
         <v>163</v>
       </c>
@@ -2997,7 +3000,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="136" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
         <v>170</v>
       </c>
@@ -3005,7 +3008,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="137" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
         <v>175</v>
       </c>
@@ -3013,7 +3016,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="138" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
         <v>180</v>
       </c>
@@ -3021,7 +3024,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="139" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
         <v>185</v>
       </c>
@@ -3029,7 +3032,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="140" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
         <v>190</v>
       </c>
@@ -3037,7 +3040,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="141" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
         <v>195</v>
       </c>
@@ -3045,7 +3048,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="142" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
         <v>200</v>
       </c>
@@ -3053,7 +3056,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="143" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
         <v>205</v>
       </c>
@@ -3061,7 +3064,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="144" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
         <v>210</v>
       </c>
@@ -3069,7 +3072,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="145" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
         <v>215</v>
       </c>
@@ -3077,7 +3080,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="146" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
         <v>220</v>
       </c>
@@ -3085,7 +3088,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="147" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
         <v>225</v>
       </c>
@@ -3093,7 +3096,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="148" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
         <v>230</v>
       </c>
@@ -3101,7 +3104,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="149" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
         <v>235</v>
       </c>
@@ -3109,7 +3112,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="150" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
         <v>240</v>
       </c>
@@ -3117,7 +3120,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="151" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
         <v>245</v>
       </c>
@@ -3125,7 +3128,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="152" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
         <v>250</v>
       </c>
@@ -3133,7 +3136,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="153" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
         <v>254</v>
       </c>
@@ -3141,7 +3144,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="154" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
         <v>258</v>
       </c>
@@ -3149,7 +3152,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="155" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
         <v>262</v>
       </c>
@@ -3157,7 +3160,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="156" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
         <v>266</v>
       </c>
@@ -3165,7 +3168,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="157" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
         <v>270</v>
       </c>
@@ -3173,7 +3176,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="158" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
         <v>274</v>
       </c>
@@ -3181,7 +3184,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="159" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
         <v>278</v>
       </c>
@@ -3189,7 +3192,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="160" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
         <v>282</v>
       </c>
@@ -3197,7 +3200,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="161" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
         <v>285</v>
       </c>
@@ -3205,7 +3208,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="162" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
         <v>288</v>
       </c>
@@ -3213,7 +3216,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="163" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
         <v>291</v>
       </c>
@@ -3221,7 +3224,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="164" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
         <v>294</v>
       </c>
@@ -3229,7 +3232,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="165" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
         <v>297</v>
       </c>
@@ -3237,7 +3240,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="166" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
         <v>300</v>
       </c>
@@ -3245,7 +3248,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="167" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
         <v>303</v>
       </c>
@@ -3253,7 +3256,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="168" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
         <v>306</v>
       </c>
@@ -3261,7 +3264,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="169" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
         <v>309</v>
       </c>
@@ -3269,7 +3272,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="170" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
         <v>312</v>
       </c>
@@ -3277,7 +3280,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="171" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
         <v>314</v>
       </c>
@@ -3285,7 +3288,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="172" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
         <v>316</v>
       </c>
@@ -3293,7 +3296,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="173" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
         <v>318</v>
       </c>
@@ -3301,7 +3304,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="174" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
         <v>320</v>
       </c>
@@ -3309,7 +3312,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="175" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
         <v>322</v>
       </c>
@@ -3317,7 +3320,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="176" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
         <v>324</v>
       </c>
@@ -3325,7 +3328,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="177" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
         <v>326</v>
       </c>
@@ -3333,7 +3336,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="178" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
         <v>328</v>
       </c>
@@ -3341,7 +3344,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="179" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
         <v>330</v>
       </c>
@@ -3349,7 +3352,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="180" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
         <v>332</v>
       </c>
@@ -3357,7 +3360,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="181" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
         <v>334</v>
       </c>
@@ -3365,7 +3368,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="182" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
         <v>336</v>
       </c>
@@ -3373,7 +3376,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="183" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="s">
         <v>338</v>
       </c>
@@ -3381,7 +3384,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="184" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
         <v>340</v>
       </c>
@@ -3389,7 +3392,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="185" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="s">
         <v>342</v>
       </c>
@@ -3397,7 +3400,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="186" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
         <v>344</v>
       </c>
@@ -3405,7 +3408,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="187" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" s="1" t="s">
         <v>346</v>
       </c>
@@ -3413,7 +3416,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="188" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
         <v>348</v>
       </c>
@@ -3421,7 +3424,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="189" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" s="1" t="s">
         <v>350</v>
       </c>
@@ -3429,7 +3432,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="190" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="s">
         <v>352</v>
       </c>
@@ -3437,7 +3440,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="191" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" s="1" t="s">
         <v>354</v>
       </c>
@@ -3445,7 +3448,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="192" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
         <v>356</v>
       </c>
@@ -3453,7 +3456,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="193" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
         <v>358</v>
       </c>
@@ -3461,7 +3464,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="194" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
         <v>360</v>
       </c>
@@ -3469,7 +3472,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="195" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" s="1" t="s">
         <v>362</v>
       </c>
@@ -3477,7 +3480,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="196" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
         <v>364</v>
       </c>
@@ -3485,7 +3488,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="197" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" s="1" t="s">
         <v>366</v>
       </c>
@@ -3493,7 +3496,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="198" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" s="1" t="s">
         <v>368</v>
       </c>
@@ -3501,7 +3504,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="199" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" s="1" t="s">
         <v>370</v>
       </c>
@@ -3509,7 +3512,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="200" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" s="1" t="s">
         <v>372</v>
       </c>
@@ -3517,7 +3520,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="201" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" s="1" t="s">
         <v>374</v>
       </c>
@@ -3525,7 +3528,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="202" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" s="1" t="s">
         <v>1</v>
       </c>
@@ -3533,7 +3536,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="203" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" s="1" t="s">
         <v>8</v>
       </c>
@@ -3541,7 +3544,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="204" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204" s="1" t="s">
         <v>15</v>
       </c>
@@ -3549,7 +3552,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="205" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" s="1" t="s">
         <v>22</v>
       </c>
@@ -3557,7 +3560,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="206" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" s="1" t="s">
         <v>29</v>
       </c>
@@ -3565,7 +3568,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="207" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" s="1" t="s">
         <v>36</v>
       </c>
@@ -3573,7 +3576,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="208" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" s="1" t="s">
         <v>43</v>
       </c>
@@ -3581,7 +3584,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="209" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209" s="1" t="s">
         <v>50</v>
       </c>
@@ -3589,7 +3592,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="210" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210" s="1" t="s">
         <v>57</v>
       </c>
@@ -3597,7 +3600,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="211" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211" s="1" t="s">
         <v>64</v>
       </c>
@@ -3605,7 +3608,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="212" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212" s="1" t="s">
         <v>71</v>
       </c>
@@ -3613,7 +3616,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="213" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213" s="1" t="s">
         <v>78</v>
       </c>
@@ -3621,7 +3624,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="214" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214" s="1" t="s">
         <v>157</v>
       </c>
@@ -3629,7 +3632,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="215" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A215" s="1" t="s">
         <v>164</v>
       </c>
@@ -3637,7 +3640,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="216" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A216" s="1" t="s">
         <v>171</v>
       </c>
@@ -3645,7 +3648,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="217" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217" s="1" t="s">
         <v>176</v>
       </c>
@@ -3653,7 +3656,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="218" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218" s="1" t="s">
         <v>181</v>
       </c>
@@ -3661,7 +3664,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="219" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A219" s="1" t="s">
         <v>186</v>
       </c>
@@ -3669,7 +3672,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="220" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220" s="1" t="s">
         <v>191</v>
       </c>
@@ -3677,7 +3680,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="221" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A221" s="1" t="s">
         <v>196</v>
       </c>
@@ -3685,7 +3688,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="222" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A222" s="1" t="s">
         <v>201</v>
       </c>
@@ -3693,7 +3696,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="223" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A223" s="1" t="s">
         <v>206</v>
       </c>
@@ -3701,7 +3704,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="224" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A224" s="1" t="s">
         <v>211</v>
       </c>
@@ -3709,7 +3712,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="225" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A225" s="1" t="s">
         <v>216</v>
       </c>
@@ -3717,7 +3720,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="226" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A226" s="1" t="s">
         <v>221</v>
       </c>
@@ -3725,7 +3728,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="227" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A227" s="1" t="s">
         <v>226</v>
       </c>
@@ -3733,7 +3736,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="228" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A228" s="1" t="s">
         <v>231</v>
       </c>
@@ -3741,7 +3744,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="229" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A229" s="1" t="s">
         <v>236</v>
       </c>
@@ -3749,7 +3752,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="230" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A230" s="1" t="s">
         <v>241</v>
       </c>
@@ -3757,7 +3760,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="231" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A231" s="1" t="s">
         <v>246</v>
       </c>
@@ -3765,7 +3768,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="232" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A232" s="1" t="s">
         <v>251</v>
       </c>
@@ -3773,7 +3776,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="233" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A233" s="1" t="s">
         <v>255</v>
       </c>
@@ -3781,7 +3784,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="234" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A234" s="1" t="s">
         <v>259</v>
       </c>
@@ -3789,7 +3792,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="235" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A235" s="1" t="s">
         <v>263</v>
       </c>
@@ -3797,7 +3800,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="236" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A236" s="1" t="s">
         <v>267</v>
       </c>
@@ -3805,7 +3808,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="237" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A237" s="1" t="s">
         <v>271</v>
       </c>
@@ -3813,7 +3816,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="238" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A238" s="1" t="s">
         <v>275</v>
       </c>
@@ -3821,7 +3824,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="239" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A239" s="1" t="s">
         <v>279</v>
       </c>
@@ -3829,7 +3832,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="240" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A240" s="1" t="s">
         <v>283</v>
       </c>
@@ -3837,7 +3840,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="241" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A241" s="1" t="s">
         <v>286</v>
       </c>
@@ -3845,7 +3848,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="242" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A242" s="1" t="s">
         <v>289</v>
       </c>
@@ -3853,7 +3856,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="243" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A243" s="1" t="s">
         <v>292</v>
       </c>
@@ -3861,7 +3864,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="244" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A244" s="1" t="s">
         <v>295</v>
       </c>
@@ -3869,7 +3872,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="245" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A245" s="1" t="s">
         <v>298</v>
       </c>
@@ -3877,7 +3880,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="246" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A246" s="1" t="s">
         <v>301</v>
       </c>
@@ -3885,7 +3888,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="247" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A247" s="1" t="s">
         <v>304</v>
       </c>
@@ -3893,7 +3896,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="248" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A248" s="1" t="s">
         <v>307</v>
       </c>
@@ -3901,7 +3904,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="249" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A249" s="1" t="s">
         <v>310</v>
       </c>
@@ -3914,7 +3917,7 @@
         <v>2</v>
       </c>
       <c r="B250" s="1" t="s">
-        <v>491</v>
+        <v>494</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.25">
@@ -3922,7 +3925,7 @@
         <v>9</v>
       </c>
       <c r="B251" s="1" t="s">
-        <v>491</v>
+        <v>494</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.25">
@@ -3930,7 +3933,7 @@
         <v>16</v>
       </c>
       <c r="B252" s="1" t="s">
-        <v>491</v>
+        <v>494</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.25">
@@ -3938,7 +3941,7 @@
         <v>23</v>
       </c>
       <c r="B253" s="1" t="s">
-        <v>491</v>
+        <v>494</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.25">
@@ -3946,7 +3949,7 @@
         <v>30</v>
       </c>
       <c r="B254" s="1" t="s">
-        <v>491</v>
+        <v>494</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.25">
@@ -3954,7 +3957,7 @@
         <v>37</v>
       </c>
       <c r="B255" s="1" t="s">
-        <v>491</v>
+        <v>494</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.25">
@@ -4106,7 +4109,7 @@
         <v>172</v>
       </c>
       <c r="B274" s="1" t="s">
-        <v>491</v>
+        <v>494</v>
       </c>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.25">
@@ -4114,7 +4117,7 @@
         <v>177</v>
       </c>
       <c r="B275" s="1" t="s">
-        <v>491</v>
+        <v>494</v>
       </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.25">
@@ -4122,7 +4125,7 @@
         <v>182</v>
       </c>
       <c r="B276" s="1" t="s">
-        <v>491</v>
+        <v>494</v>
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.25">
@@ -4130,7 +4133,7 @@
         <v>187</v>
       </c>
       <c r="B277" s="1" t="s">
-        <v>491</v>
+        <v>494</v>
       </c>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.25">
@@ -4138,7 +4141,7 @@
         <v>192</v>
       </c>
       <c r="B278" s="1" t="s">
-        <v>491</v>
+        <v>494</v>
       </c>
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.25">
@@ -4146,7 +4149,7 @@
         <v>197</v>
       </c>
       <c r="B279" s="1" t="s">
-        <v>491</v>
+        <v>494</v>
       </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.25">
@@ -4293,7 +4296,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="298" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A298" s="1" t="s">
         <v>4</v>
       </c>
@@ -4301,7 +4304,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="299" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A299" s="1" t="s">
         <v>11</v>
       </c>
@@ -4309,7 +4312,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="300" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A300" s="1" t="s">
         <v>18</v>
       </c>
@@ -4317,7 +4320,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="301" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A301" s="1" t="s">
         <v>25</v>
       </c>
@@ -4325,7 +4328,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="302" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A302" s="1" t="s">
         <v>32</v>
       </c>
@@ -4333,7 +4336,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="303" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A303" s="1" t="s">
         <v>39</v>
       </c>
@@ -4341,7 +4344,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="304" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A304" s="1" t="s">
         <v>46</v>
       </c>
@@ -4349,7 +4352,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="305" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A305" s="1" t="s">
         <v>53</v>
       </c>
@@ -4357,7 +4360,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="306" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A306" s="1" t="s">
         <v>60</v>
       </c>
@@ -4365,7 +4368,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="307" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A307" s="1" t="s">
         <v>67</v>
       </c>
@@ -4373,7 +4376,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="308" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A308" s="1" t="s">
         <v>74</v>
       </c>
@@ -4381,7 +4384,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="309" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A309" s="1" t="s">
         <v>81</v>
       </c>
@@ -4389,7 +4392,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="310" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A310" s="1" t="s">
         <v>89</v>
       </c>
@@ -4397,7 +4400,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="311" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A311" s="1" t="s">
         <v>97</v>
       </c>
@@ -4405,7 +4408,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="312" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A312" s="1" t="s">
         <v>493</v>
       </c>
@@ -4413,7 +4416,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="313" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A313" s="1" t="s">
         <v>111</v>
       </c>
@@ -4421,7 +4424,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="314" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A314" s="1" t="s">
         <v>118</v>
       </c>
@@ -4429,7 +4432,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="315" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A315" s="1" t="s">
         <v>125</v>
       </c>
@@ -4437,7 +4440,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="316" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A316" s="1" t="s">
         <v>132</v>
       </c>
@@ -4445,7 +4448,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="317" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A317" s="1" t="s">
         <v>139</v>
       </c>
@@ -4453,7 +4456,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="318" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A318" s="1" t="s">
         <v>146</v>
       </c>
@@ -4461,7 +4464,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="319" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A319" s="1" t="s">
         <v>153</v>
       </c>
@@ -4469,7 +4472,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="320" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A320" s="1" t="s">
         <v>160</v>
       </c>
@@ -4477,7 +4480,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="321" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A321" s="1" t="s">
         <v>167</v>
       </c>
@@ -4485,7 +4488,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="322" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A322" s="1" t="s">
         <v>174</v>
       </c>
@@ -4493,7 +4496,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="323" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A323" s="1" t="s">
         <v>179</v>
       </c>
@@ -4501,7 +4504,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="324" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A324" s="1" t="s">
         <v>184</v>
       </c>
@@ -4509,7 +4512,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="325" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A325" s="1" t="s">
         <v>189</v>
       </c>
@@ -4517,7 +4520,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="326" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A326" s="1" t="s">
         <v>194</v>
       </c>
@@ -4525,7 +4528,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="327" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A327" s="1" t="s">
         <v>199</v>
       </c>
@@ -4533,7 +4536,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="328" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A328" s="1" t="s">
         <v>204</v>
       </c>
@@ -4541,7 +4544,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="329" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A329" s="1" t="s">
         <v>209</v>
       </c>
@@ -4549,7 +4552,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="330" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A330" s="1" t="s">
         <v>214</v>
       </c>
@@ -4557,7 +4560,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="331" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A331" s="1" t="s">
         <v>219</v>
       </c>
@@ -4565,7 +4568,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="332" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A332" s="1" t="s">
         <v>224</v>
       </c>
@@ -4573,7 +4576,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="333" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A333" s="1" t="s">
         <v>229</v>
       </c>
@@ -4901,7 +4904,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="374" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A374" s="1" t="s">
         <v>86</v>
       </c>
@@ -4909,7 +4912,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="375" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A375" s="1" t="s">
         <v>94</v>
       </c>
@@ -4917,7 +4920,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="376" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A376" s="1" t="s">
         <v>102</v>
       </c>
@@ -4925,7 +4928,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="377" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A377" s="1" t="s">
         <v>108</v>
       </c>
@@ -4933,7 +4936,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="378" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A378" s="1" t="s">
         <v>115</v>
       </c>
@@ -4941,7 +4944,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="379" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A379" s="1" t="s">
         <v>122</v>
       </c>
@@ -4949,7 +4952,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="380" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A380" s="1" t="s">
         <v>129</v>
       </c>
@@ -4957,7 +4960,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="381" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A381" s="1" t="s">
         <v>136</v>
       </c>
@@ -4965,7 +4968,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="382" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A382" s="1" t="s">
         <v>143</v>
       </c>
@@ -4973,7 +4976,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="383" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A383" s="1" t="s">
         <v>150</v>
       </c>
@@ -4981,7 +4984,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="384" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A384" s="1" t="s">
         <v>384</v>
       </c>
@@ -4989,7 +4992,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="385" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A385" s="1" t="s">
         <v>385</v>
       </c>
@@ -4997,7 +5000,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="386" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A386" s="1" t="s">
         <v>386</v>
       </c>
@@ -5005,7 +5008,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="387" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A387" s="1" t="s">
         <v>387</v>
       </c>
@@ -5013,7 +5016,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="388" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A388" s="1" t="s">
         <v>388</v>
       </c>
@@ -5021,7 +5024,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="389" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A389" s="1" t="s">
         <v>389</v>
       </c>
@@ -5029,7 +5032,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="390" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A390" s="1" t="s">
         <v>390</v>
       </c>
@@ -5037,7 +5040,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="391" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A391" s="1" t="s">
         <v>391</v>
       </c>
@@ -5045,7 +5048,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="392" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A392" s="1" t="s">
         <v>392</v>
       </c>
@@ -5053,7 +5056,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="393" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A393" s="1" t="s">
         <v>393</v>
       </c>
@@ -5061,7 +5064,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="394" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A394" s="1" t="s">
         <v>394</v>
       </c>
@@ -5069,7 +5072,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="395" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A395" s="1" t="s">
         <v>395</v>
       </c>
@@ -5077,7 +5080,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="396" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A396" s="1" t="s">
         <v>5</v>
       </c>
@@ -5085,7 +5088,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="397" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A397" s="1" t="s">
         <v>12</v>
       </c>
@@ -5093,7 +5096,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="398" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A398" s="1" t="s">
         <v>19</v>
       </c>
@@ -5101,7 +5104,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="399" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A399" s="1" t="s">
         <v>26</v>
       </c>
@@ -5109,7 +5112,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="400" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A400" s="1" t="s">
         <v>33</v>
       </c>
@@ -5117,7 +5120,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="401" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A401" s="1" t="s">
         <v>40</v>
       </c>
@@ -5125,7 +5128,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="402" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A402" s="1" t="s">
         <v>47</v>
       </c>
@@ -5133,7 +5136,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="403" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A403" s="1" t="s">
         <v>54</v>
       </c>
@@ -5141,7 +5144,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="404" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A404" s="1" t="s">
         <v>61</v>
       </c>
@@ -5149,7 +5152,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="405" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A405" s="1" t="s">
         <v>68</v>
       </c>
@@ -5157,7 +5160,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="406" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A406" s="1" t="s">
         <v>75</v>
       </c>
@@ -5165,7 +5168,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="407" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A407" s="1" t="s">
         <v>82</v>
       </c>
@@ -5173,7 +5176,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="408" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A408" s="1" t="s">
         <v>90</v>
       </c>
@@ -5181,7 +5184,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="409" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A409" s="1" t="s">
         <v>98</v>
       </c>
@@ -5189,7 +5192,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="410" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A410" s="1" t="s">
         <v>105</v>
       </c>
@@ -5197,7 +5200,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="411" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A411" s="1" t="s">
         <v>112</v>
       </c>
@@ -5205,7 +5208,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="412" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A412" s="1" t="s">
         <v>119</v>
       </c>
@@ -5213,7 +5216,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="413" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A413" s="1" t="s">
         <v>126</v>
       </c>
@@ -5221,7 +5224,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="414" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A414" s="1" t="s">
         <v>133</v>
       </c>
@@ -5229,7 +5232,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="415" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A415" s="1" t="s">
         <v>140</v>
       </c>
@@ -5237,7 +5240,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="416" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A416" s="1" t="s">
         <v>147</v>
       </c>
@@ -5245,7 +5248,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="417" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A417" s="1" t="s">
         <v>154</v>
       </c>
@@ -5253,7 +5256,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="418" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A418" s="1" t="s">
         <v>161</v>
       </c>
@@ -5261,7 +5264,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="419" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A419" s="1" t="s">
         <v>168</v>
       </c>
@@ -5269,7 +5272,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="420" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A420" s="1" t="s">
         <v>6</v>
       </c>
@@ -5277,7 +5280,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="421" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A421" s="1" t="s">
         <v>13</v>
       </c>
@@ -5285,7 +5288,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="422" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A422" s="1" t="s">
         <v>20</v>
       </c>
@@ -5293,7 +5296,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="423" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A423" s="1" t="s">
         <v>27</v>
       </c>
@@ -5301,7 +5304,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="424" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A424" s="1" t="s">
         <v>34</v>
       </c>
@@ -5309,7 +5312,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="425" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A425" s="1" t="s">
         <v>41</v>
       </c>
@@ -5317,7 +5320,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="426" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A426" s="1" t="s">
         <v>48</v>
       </c>
@@ -5325,7 +5328,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="427" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A427" s="1" t="s">
         <v>55</v>
       </c>
@@ -5333,7 +5336,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="428" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A428" s="1" t="s">
         <v>62</v>
       </c>
@@ -5341,7 +5344,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="429" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A429" s="1" t="s">
         <v>69</v>
       </c>
@@ -5349,7 +5352,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="430" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A430" s="1" t="s">
         <v>76</v>
       </c>
@@ -5357,7 +5360,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="431" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A431" s="1" t="s">
         <v>83</v>
       </c>
@@ -5365,7 +5368,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="432" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A432" s="1" t="s">
         <v>91</v>
       </c>
@@ -5373,7 +5376,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="433" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A433" s="1" t="s">
         <v>99</v>
       </c>
@@ -5381,7 +5384,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="434" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A434" s="3" t="s">
         <v>414</v>
       </c>
@@ -5389,7 +5392,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="435" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A435" s="3" t="s">
         <v>415</v>
       </c>
@@ -5397,7 +5400,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="436" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A436" s="3" t="s">
         <v>416</v>
       </c>
@@ -5405,7 +5408,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="437" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A437" s="3" t="s">
         <v>417</v>
       </c>
@@ -5413,7 +5416,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="438" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A438" s="3" t="s">
         <v>418</v>
       </c>
@@ -5421,7 +5424,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="439" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A439" s="3" t="s">
         <v>419</v>
       </c>
@@ -5429,7 +5432,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="440" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A440" s="3" t="s">
         <v>420</v>
       </c>
@@ -5437,7 +5440,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="441" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A441" s="3" t="s">
         <v>421</v>
       </c>
@@ -5445,7 +5448,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="442" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A442" s="3" t="s">
         <v>422</v>
       </c>
@@ -5453,7 +5456,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="443" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A443" s="3" t="s">
         <v>423</v>
       </c>
@@ -5461,7 +5464,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="444" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A444" s="3" t="s">
         <v>424</v>
       </c>
@@ -5469,7 +5472,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="445" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A445" s="3" t="s">
         <v>425</v>
       </c>
@@ -5477,7 +5480,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="446" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A446" s="3" t="s">
         <v>426</v>
       </c>
@@ -5485,7 +5488,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="447" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A447" s="3" t="s">
         <v>427</v>
       </c>
@@ -5493,7 +5496,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="448" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A448" s="3" t="s">
         <v>428</v>
       </c>
@@ -5501,7 +5504,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="449" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A449" s="3" t="s">
         <v>429</v>
       </c>
@@ -5509,7 +5512,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="450" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A450" s="3" t="s">
         <v>430</v>
       </c>
@@ -5517,7 +5520,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="451" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A451" s="3" t="s">
         <v>431</v>
       </c>
@@ -5525,7 +5528,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="452" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A452" s="3" t="s">
         <v>432</v>
       </c>
@@ -5533,7 +5536,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="453" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A453" s="3" t="s">
         <v>433</v>
       </c>
@@ -5541,7 +5544,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="454" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A454" s="3" t="s">
         <v>434</v>
       </c>
@@ -5549,7 +5552,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="455" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A455" s="3" t="s">
         <v>435</v>
       </c>
@@ -5557,7 +5560,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="456" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A456" s="3" t="s">
         <v>436</v>
       </c>
@@ -5565,7 +5568,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="457" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A457" s="3" t="s">
         <v>437</v>
       </c>
@@ -5573,7 +5576,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="458" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A458" s="3" t="s">
         <v>438</v>
       </c>
@@ -5581,7 +5584,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="459" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A459" s="3" t="s">
         <v>439</v>
       </c>
@@ -5589,7 +5592,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="460" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A460" s="3" t="s">
         <v>440</v>
       </c>
@@ -5597,7 +5600,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="461" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A461" s="3" t="s">
         <v>441</v>
       </c>
@@ -5605,7 +5608,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="462" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A462" s="3" t="s">
         <v>442</v>
       </c>
@@ -5613,7 +5616,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="463" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A463" s="3" t="s">
         <v>443</v>
       </c>
@@ -5621,7 +5624,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="464" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A464" s="3" t="s">
         <v>444</v>
       </c>
@@ -5629,7 +5632,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="465" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A465" s="3" t="s">
         <v>445</v>
       </c>
@@ -5637,7 +5640,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="466" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="466" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A466" s="3" t="s">
         <v>446</v>
       </c>
@@ -5645,7 +5648,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="467" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="467" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A467" s="3" t="s">
         <v>398</v>
       </c>
@@ -5653,7 +5656,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="468" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="468" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A468" s="3" t="s">
         <v>399</v>
       </c>
@@ -5661,7 +5664,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="469" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="469" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A469" s="3" t="s">
         <v>400</v>
       </c>
@@ -5669,7 +5672,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="470" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="470" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A470" s="3" t="s">
         <v>401</v>
       </c>
@@ -5677,7 +5680,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="471" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="471" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A471" s="3" t="s">
         <v>402</v>
       </c>
@@ -5685,7 +5688,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="472" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="472" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A472" s="3" t="s">
         <v>403</v>
       </c>
@@ -5693,7 +5696,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="473" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="473" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A473" s="3" t="s">
         <v>404</v>
       </c>
@@ -5701,7 +5704,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="474" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="474" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A474" s="3" t="s">
         <v>405</v>
       </c>
@@ -5709,7 +5712,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="475" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="475" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A475" s="3" t="s">
         <v>406</v>
       </c>
@@ -5717,7 +5720,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="476" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="476" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A476" s="3" t="s">
         <v>407</v>
       </c>
@@ -5725,7 +5728,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="477" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="477" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A477" s="3" t="s">
         <v>408</v>
       </c>
@@ -5733,7 +5736,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="478" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="478" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A478" s="3" t="s">
         <v>409</v>
       </c>
@@ -5741,7 +5744,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="479" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="479" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A479" s="3" t="s">
         <v>410</v>
       </c>
@@ -5749,7 +5752,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="480" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="480" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A480" s="3" t="s">
         <v>411</v>
       </c>
@@ -5757,7 +5760,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="481" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="481" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A481" s="3" t="s">
         <v>412</v>
       </c>
@@ -5765,7 +5768,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="482" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="482" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A482" s="3" t="s">
         <v>413</v>
       </c>
@@ -5774,13 +5777,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B482" xr:uid="{E3722E28-546D-45F9-BF38-B4D5FA1D8738}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="apanha_b"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:B482" xr:uid="{E3722E28-546D-45F9-BF38-B4D5FA1D8738}"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
atualizando orientação e local de apanha cx
</commit_message>
<xml_diff>
--- a/data/analise_curva_abc/local/datasets/local_apanha_cx.xlsx
+++ b/data/analise_curva_abc/local/datasets/local_apanha_cx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://maxifarmabr-my.sharepoint.com/personal/controle_estoque_grupomaxifarma_com_br/Documents/Documentos/estoque.renan/projetos/projeto_curva_abc/data/analise_curva_abc/local/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="73" documentId="13_ncr:1_{62563889-610E-48F9-917B-CDA4FE3D6C5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FC5E2E46-8D33-4EB4-BD07-0C29DCBD3978}"/>
+  <xr:revisionPtr revIDLastSave="75" documentId="13_ncr:1_{62563889-610E-48F9-917B-CDA4FE3D6C5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{79B849A0-1789-4281-BAE2-FCAB6589C4BE}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{18EFAD8D-C71D-455A-9E0F-2475F39BFCF9}"/>
   </bookViews>
@@ -1909,7 +1909,7 @@
   <dimension ref="A1:F482"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>